<commit_message>
update some errors in two lists
</commit_message>
<xml_diff>
--- a/data/Eksklusionslister/PenSam_eksklusionsliste_isin.xlsx
+++ b/data/Eksklusionslister/PenSam_eksklusionsliste_isin.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="27928"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="28025"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Anja\Documents\Python_projekter\kommune_investering\data\Eksklusionslister\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Anja\OneDrive - Gravercentret\Dokumenter\Python_projekter\kommune_investering\data\Eksklusionslister\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CD2FD6FB-F382-4AD1-A7B0-67A36D67AB53}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E0F46520-6EA2-468E-91DC-C5B573A57013}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="14295" yWindow="0" windowWidth="14610" windowHeight="15585" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2802" uniqueCount="921">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2802" uniqueCount="920">
   <si>
     <t>Selskab</t>
   </si>
@@ -2431,9 +2431,6 @@
     <t>['US6745991058']</t>
   </si>
   <si>
-    <t>['AT0000743059', 'US98980L1017', 'XS2224439385', 'XS2240463674']</t>
-  </si>
-  <si>
     <t>['USG82016AT66']</t>
   </si>
   <si>
@@ -2566,9 +2563,6 @@
     <t>['OCCIDENTAL PETROLEUM CORPORATION']</t>
   </si>
   <si>
-    <t>['OMV AG', nan, 'Zoom Video Communications Inc', 'USA', 'Zoom Video Communications Inc. A', 'Zoom\xa0Video\xa0Communications\xa0Inc', 'EU', 'OMV AG ', 'Østrig', 'Lorca Telecom Virksomhedsobligationco SAU 18.09.2027']</t>
-  </si>
-  <si>
     <t>['Sinopec Group Overseas Development 2018 Ltd']</t>
   </si>
   <si>
@@ -2659,9 +2653,6 @@
     <t>['Occidental Petroleum Corp']</t>
   </si>
   <si>
-    <t>['OMV AG', 'Zoom Video Communications', 'Zoom Video Communications Inc', 'Zoom Video Communications Inc. A', 'Zoom Video Communications, Inc.', 'ZOOM VIDEO COMMUNICATIONS-A', 'Zoom\xa0Video\xa0Communications', 'OMV AG PERP', 'LORCAT 4 09/18/27']</t>
-  </si>
-  <si>
     <t>['3,1 SINOPE 08-01-2051 (REGS)']</t>
   </si>
   <si>
@@ -2752,9 +2743,6 @@
     <t>['Rødovre', 'Norddjurs']</t>
   </si>
   <si>
-    <t>['Rødovre', 'Næstved', 'Odense', 'Randers', 'Faaborg-Midtfyn', 'Guldborgsund', 'Hedensted', 'Helsingør', 'Hørsholm', 'Middelfart', 'Norddjurs', 'Nordfyn', 'Roskilde', 'Slagelse', 'Svendborg', 'Syddjurs', 'Holstebro', 'Ikast-Brande', 'Esbjerg', 'Aalborg', 'Fanø', 'Aarhus', 'Mariagerfjord', 'Fredericia', 'Greve', 'Herning', 'Hillerød', 'Høje Taastrup', 'Kolding', 'Lemvig', 'Skive', 'Varde', 'Aabenraa', 'Region\xa0Nordjylland', 'Viborg', 'Kalundborg', 'Vejen']</t>
-  </si>
-  <si>
     <t>['Rødovre', 'Skive', 'Svendborg', 'Kalundborg', 'Fanø', 'Vejen', 'Holbæk']</t>
   </si>
   <si>
@@ -2783,6 +2771,15 @@
   </si>
   <si>
     <t>['Hess Corp.', 'HESS MIDSTREAM OPERATIONS LP', 'Hess Midstream Operations LP']</t>
+  </si>
+  <si>
+    <t>['OMV AG', nan, 'OMV AG ', 'Østrig', 'Lorca Telecom Virksomhedsobligationco SAU 18.09.2027']</t>
+  </si>
+  <si>
+    <t>['OMV AG', 'OMV AG PERP', 'LORCAT 4 09/18/27']</t>
+  </si>
+  <si>
+    <t>['AT0000743059',  'XS2224439385']</t>
   </si>
 </sst>
 </file>
@@ -3159,13 +3156,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:I351"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A319" workbookViewId="0">
-      <selection activeCell="L328" sqref="L328"/>
+    <sheetView tabSelected="1" topLeftCell="A298" workbookViewId="0">
+      <selection activeCell="F310" sqref="F310"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="54" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="162.77734375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="200.88671875" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -3194,7 +3196,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>9</v>
       </c>
@@ -3223,7 +3225,7 @@
         <v>760</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>10</v>
       </c>
@@ -3252,7 +3254,7 @@
         <v>760</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>11</v>
       </c>
@@ -3272,16 +3274,16 @@
         <v>761</v>
       </c>
       <c r="G4" t="s">
-        <v>806</v>
+        <v>805</v>
       </c>
       <c r="H4" t="s">
-        <v>851</v>
+        <v>849</v>
       </c>
       <c r="I4" t="s">
-        <v>882</v>
-      </c>
-    </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+        <v>879</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>12</v>
       </c>
@@ -3310,7 +3312,7 @@
         <v>760</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>13</v>
       </c>
@@ -3339,7 +3341,7 @@
         <v>760</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>14</v>
       </c>
@@ -3368,7 +3370,7 @@
         <v>760</v>
       </c>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>15</v>
       </c>
@@ -3397,7 +3399,7 @@
         <v>760</v>
       </c>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>16</v>
       </c>
@@ -3417,16 +3419,16 @@
         <v>762</v>
       </c>
       <c r="G9" t="s">
-        <v>807</v>
+        <v>806</v>
       </c>
       <c r="H9" t="s">
-        <v>852</v>
+        <v>850</v>
       </c>
       <c r="I9" t="s">
-        <v>883</v>
-      </c>
-    </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+        <v>880</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>17</v>
       </c>
@@ -3446,16 +3448,16 @@
         <v>763</v>
       </c>
       <c r="G10" t="s">
-        <v>808</v>
+        <v>807</v>
       </c>
       <c r="H10" t="s">
-        <v>853</v>
+        <v>851</v>
       </c>
       <c r="I10" t="s">
-        <v>884</v>
-      </c>
-    </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+        <v>881</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A11" s="2" t="s">
         <v>18</v>
       </c>
@@ -3472,19 +3474,19 @@
         <v>420</v>
       </c>
       <c r="F11" s="2" t="s">
-        <v>912</v>
+        <v>908</v>
       </c>
       <c r="G11" s="2" t="s">
-        <v>913</v>
+        <v>909</v>
       </c>
       <c r="H11" t="s">
         <v>760</v>
       </c>
       <c r="I11" s="2" t="s">
-        <v>885</v>
-      </c>
-    </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+        <v>882</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>19</v>
       </c>
@@ -3513,7 +3515,7 @@
         <v>760</v>
       </c>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>20</v>
       </c>
@@ -3533,16 +3535,16 @@
         <v>764</v>
       </c>
       <c r="G13" t="s">
-        <v>809</v>
+        <v>808</v>
       </c>
       <c r="H13" t="s">
-        <v>854</v>
+        <v>852</v>
       </c>
       <c r="I13" t="s">
-        <v>886</v>
-      </c>
-    </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
+        <v>883</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>21</v>
       </c>
@@ -3562,16 +3564,16 @@
         <v>765</v>
       </c>
       <c r="G14" t="s">
-        <v>810</v>
+        <v>809</v>
       </c>
       <c r="H14" t="s">
-        <v>855</v>
+        <v>853</v>
       </c>
       <c r="I14" t="s">
-        <v>887</v>
-      </c>
-    </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
+        <v>884</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>22</v>
       </c>
@@ -3588,7 +3590,7 @@
         <v>424</v>
       </c>
       <c r="F15" t="s">
-        <v>914</v>
+        <v>910</v>
       </c>
       <c r="G15" t="s">
         <v>760</v>
@@ -3600,7 +3602,7 @@
         <v>760</v>
       </c>
     </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>23</v>
       </c>
@@ -3629,7 +3631,7 @@
         <v>760</v>
       </c>
     </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>24</v>
       </c>
@@ -3658,7 +3660,7 @@
         <v>760</v>
       </c>
     </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>25</v>
       </c>
@@ -3687,7 +3689,7 @@
         <v>760</v>
       </c>
     </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>26</v>
       </c>
@@ -3716,7 +3718,7 @@
         <v>760</v>
       </c>
     </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>27</v>
       </c>
@@ -3745,7 +3747,7 @@
         <v>760</v>
       </c>
     </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
         <v>28</v>
       </c>
@@ -3774,7 +3776,7 @@
         <v>760</v>
       </c>
     </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
         <v>29</v>
       </c>
@@ -3803,7 +3805,7 @@
         <v>760</v>
       </c>
     </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
         <v>30</v>
       </c>
@@ -3832,7 +3834,7 @@
         <v>760</v>
       </c>
     </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
         <v>31</v>
       </c>
@@ -3861,7 +3863,7 @@
         <v>760</v>
       </c>
     </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
         <v>32</v>
       </c>
@@ -3890,7 +3892,7 @@
         <v>760</v>
       </c>
     </row>
-    <row r="26" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
         <v>33</v>
       </c>
@@ -3910,16 +3912,16 @@
         <v>766</v>
       </c>
       <c r="G26" t="s">
-        <v>811</v>
+        <v>810</v>
       </c>
       <c r="H26" t="s">
-        <v>811</v>
+        <v>810</v>
       </c>
       <c r="I26" t="s">
-        <v>888</v>
-      </c>
-    </row>
-    <row r="27" spans="1:9" x14ac:dyDescent="0.25">
+        <v>885</v>
+      </c>
+    </row>
+    <row r="27" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
         <v>34</v>
       </c>
@@ -3948,7 +3950,7 @@
         <v>760</v>
       </c>
     </row>
-    <row r="28" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
         <v>35</v>
       </c>
@@ -3977,7 +3979,7 @@
         <v>760</v>
       </c>
     </row>
-    <row r="29" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
         <v>36</v>
       </c>
@@ -4006,7 +4008,7 @@
         <v>760</v>
       </c>
     </row>
-    <row r="30" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
         <v>37</v>
       </c>
@@ -4035,7 +4037,7 @@
         <v>760</v>
       </c>
     </row>
-    <row r="31" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
         <v>38</v>
       </c>
@@ -4064,7 +4066,7 @@
         <v>760</v>
       </c>
     </row>
-    <row r="32" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
         <v>39</v>
       </c>
@@ -4084,16 +4086,16 @@
         <v>767</v>
       </c>
       <c r="G32" t="s">
-        <v>812</v>
+        <v>811</v>
       </c>
       <c r="H32" t="s">
-        <v>812</v>
+        <v>811</v>
       </c>
       <c r="I32" t="s">
-        <v>889</v>
-      </c>
-    </row>
-    <row r="33" spans="1:9" x14ac:dyDescent="0.25">
+        <v>886</v>
+      </c>
+    </row>
+    <row r="33" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
         <v>40</v>
       </c>
@@ -4122,7 +4124,7 @@
         <v>760</v>
       </c>
     </row>
-    <row r="34" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
         <v>41</v>
       </c>
@@ -4151,7 +4153,7 @@
         <v>760</v>
       </c>
     </row>
-    <row r="35" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
         <v>42</v>
       </c>
@@ -4180,7 +4182,7 @@
         <v>760</v>
       </c>
     </row>
-    <row r="36" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
         <v>43</v>
       </c>
@@ -4209,7 +4211,7 @@
         <v>760</v>
       </c>
     </row>
-    <row r="37" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
         <v>44</v>
       </c>
@@ -4238,7 +4240,7 @@
         <v>760</v>
       </c>
     </row>
-    <row r="38" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
         <v>45</v>
       </c>
@@ -4267,7 +4269,7 @@
         <v>760</v>
       </c>
     </row>
-    <row r="39" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
         <v>46</v>
       </c>
@@ -4296,7 +4298,7 @@
         <v>760</v>
       </c>
     </row>
-    <row r="40" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
         <v>47</v>
       </c>
@@ -4325,7 +4327,7 @@
         <v>760</v>
       </c>
     </row>
-    <row r="41" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A41" t="s">
         <v>48</v>
       </c>
@@ -4345,16 +4347,16 @@
         <v>768</v>
       </c>
       <c r="G41" t="s">
-        <v>813</v>
+        <v>812</v>
       </c>
       <c r="H41" t="s">
-        <v>813</v>
+        <v>812</v>
       </c>
       <c r="I41" t="s">
-        <v>890</v>
-      </c>
-    </row>
-    <row r="42" spans="1:9" x14ac:dyDescent="0.25">
+        <v>887</v>
+      </c>
+    </row>
+    <row r="42" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A42" t="s">
         <v>49</v>
       </c>
@@ -4383,7 +4385,7 @@
         <v>760</v>
       </c>
     </row>
-    <row r="43" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A43" t="s">
         <v>50</v>
       </c>
@@ -4412,7 +4414,7 @@
         <v>760</v>
       </c>
     </row>
-    <row r="44" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A44" t="s">
         <v>51</v>
       </c>
@@ -4441,7 +4443,7 @@
         <v>760</v>
       </c>
     </row>
-    <row r="45" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A45" t="s">
         <v>52</v>
       </c>
@@ -4470,7 +4472,7 @@
         <v>760</v>
       </c>
     </row>
-    <row r="46" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A46" t="s">
         <v>53</v>
       </c>
@@ -4499,7 +4501,7 @@
         <v>760</v>
       </c>
     </row>
-    <row r="47" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A47" t="s">
         <v>54</v>
       </c>
@@ -4528,7 +4530,7 @@
         <v>760</v>
       </c>
     </row>
-    <row r="48" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A48" t="s">
         <v>55</v>
       </c>
@@ -4557,7 +4559,7 @@
         <v>760</v>
       </c>
     </row>
-    <row r="49" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A49" t="s">
         <v>56</v>
       </c>
@@ -4586,7 +4588,7 @@
         <v>760</v>
       </c>
     </row>
-    <row r="50" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A50" t="s">
         <v>57</v>
       </c>
@@ -4615,7 +4617,7 @@
         <v>760</v>
       </c>
     </row>
-    <row r="51" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A51" t="s">
         <v>58</v>
       </c>
@@ -4644,7 +4646,7 @@
         <v>760</v>
       </c>
     </row>
-    <row r="52" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A52" t="s">
         <v>59</v>
       </c>
@@ -4664,16 +4666,16 @@
         <v>769</v>
       </c>
       <c r="G52" t="s">
-        <v>814</v>
+        <v>813</v>
       </c>
       <c r="H52" t="s">
-        <v>814</v>
+        <v>813</v>
       </c>
       <c r="I52" t="s">
-        <v>891</v>
-      </c>
-    </row>
-    <row r="53" spans="1:9" x14ac:dyDescent="0.25">
+        <v>888</v>
+      </c>
+    </row>
+    <row r="53" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A53" t="s">
         <v>60</v>
       </c>
@@ -4693,16 +4695,16 @@
         <v>770</v>
       </c>
       <c r="G53" t="s">
-        <v>815</v>
+        <v>814</v>
       </c>
       <c r="H53" t="s">
-        <v>856</v>
+        <v>854</v>
       </c>
       <c r="I53" t="s">
-        <v>892</v>
-      </c>
-    </row>
-    <row r="54" spans="1:9" x14ac:dyDescent="0.25">
+        <v>889</v>
+      </c>
+    </row>
+    <row r="54" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A54" t="s">
         <v>61</v>
       </c>
@@ -4731,7 +4733,7 @@
         <v>760</v>
       </c>
     </row>
-    <row r="55" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A55" t="s">
         <v>62</v>
       </c>
@@ -4751,16 +4753,16 @@
         <v>771</v>
       </c>
       <c r="G55" t="s">
-        <v>816</v>
+        <v>815</v>
       </c>
       <c r="H55" t="s">
-        <v>857</v>
+        <v>855</v>
       </c>
       <c r="I55" t="s">
-        <v>893</v>
-      </c>
-    </row>
-    <row r="56" spans="1:9" x14ac:dyDescent="0.25">
+        <v>890</v>
+      </c>
+    </row>
+    <row r="56" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A56" t="s">
         <v>63</v>
       </c>
@@ -4789,7 +4791,7 @@
         <v>760</v>
       </c>
     </row>
-    <row r="57" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A57" t="s">
         <v>64</v>
       </c>
@@ -4818,7 +4820,7 @@
         <v>760</v>
       </c>
     </row>
-    <row r="58" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A58" t="s">
         <v>65</v>
       </c>
@@ -4847,7 +4849,7 @@
         <v>760</v>
       </c>
     </row>
-    <row r="59" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A59" t="s">
         <v>66</v>
       </c>
@@ -4876,7 +4878,7 @@
         <v>760</v>
       </c>
     </row>
-    <row r="60" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A60" t="s">
         <v>67</v>
       </c>
@@ -4905,7 +4907,7 @@
         <v>760</v>
       </c>
     </row>
-    <row r="61" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A61" t="s">
         <v>68</v>
       </c>
@@ -4934,7 +4936,7 @@
         <v>760</v>
       </c>
     </row>
-    <row r="62" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A62" t="s">
         <v>69</v>
       </c>
@@ -4963,7 +4965,7 @@
         <v>760</v>
       </c>
     </row>
-    <row r="63" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A63" t="s">
         <v>70</v>
       </c>
@@ -4992,7 +4994,7 @@
         <v>760</v>
       </c>
     </row>
-    <row r="64" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A64" t="s">
         <v>71</v>
       </c>
@@ -5021,7 +5023,7 @@
         <v>760</v>
       </c>
     </row>
-    <row r="65" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A65" t="s">
         <v>72</v>
       </c>
@@ -5050,7 +5052,7 @@
         <v>760</v>
       </c>
     </row>
-    <row r="66" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A66" t="s">
         <v>73</v>
       </c>
@@ -5079,7 +5081,7 @@
         <v>760</v>
       </c>
     </row>
-    <row r="67" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A67" t="s">
         <v>74</v>
       </c>
@@ -5108,7 +5110,7 @@
         <v>760</v>
       </c>
     </row>
-    <row r="68" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A68" t="s">
         <v>75</v>
       </c>
@@ -5137,7 +5139,7 @@
         <v>760</v>
       </c>
     </row>
-    <row r="69" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A69" t="s">
         <v>76</v>
       </c>
@@ -5166,7 +5168,7 @@
         <v>760</v>
       </c>
     </row>
-    <row r="70" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A70" t="s">
         <v>77</v>
       </c>
@@ -5195,7 +5197,7 @@
         <v>760</v>
       </c>
     </row>
-    <row r="71" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A71" t="s">
         <v>78</v>
       </c>
@@ -5224,7 +5226,7 @@
         <v>760</v>
       </c>
     </row>
-    <row r="72" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A72" t="s">
         <v>79</v>
       </c>
@@ -5253,7 +5255,7 @@
         <v>760</v>
       </c>
     </row>
-    <row r="73" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A73" t="s">
         <v>80</v>
       </c>
@@ -5282,7 +5284,7 @@
         <v>760</v>
       </c>
     </row>
-    <row r="74" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A74" t="s">
         <v>81</v>
       </c>
@@ -5311,7 +5313,7 @@
         <v>760</v>
       </c>
     </row>
-    <row r="75" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A75" t="s">
         <v>82</v>
       </c>
@@ -5340,7 +5342,7 @@
         <v>760</v>
       </c>
     </row>
-    <row r="76" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A76" t="s">
         <v>83</v>
       </c>
@@ -5369,7 +5371,7 @@
         <v>760</v>
       </c>
     </row>
-    <row r="77" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A77" t="s">
         <v>84</v>
       </c>
@@ -5398,7 +5400,7 @@
         <v>760</v>
       </c>
     </row>
-    <row r="78" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A78" t="s">
         <v>85</v>
       </c>
@@ -5427,7 +5429,7 @@
         <v>760</v>
       </c>
     </row>
-    <row r="79" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A79" t="s">
         <v>86</v>
       </c>
@@ -5456,7 +5458,7 @@
         <v>760</v>
       </c>
     </row>
-    <row r="80" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A80" t="s">
         <v>87</v>
       </c>
@@ -5485,7 +5487,7 @@
         <v>760</v>
       </c>
     </row>
-    <row r="81" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A81" t="s">
         <v>88</v>
       </c>
@@ -5514,7 +5516,7 @@
         <v>760</v>
       </c>
     </row>
-    <row r="82" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A82" t="s">
         <v>89</v>
       </c>
@@ -5543,7 +5545,7 @@
         <v>760</v>
       </c>
     </row>
-    <row r="83" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A83" t="s">
         <v>90</v>
       </c>
@@ -5572,7 +5574,7 @@
         <v>760</v>
       </c>
     </row>
-    <row r="84" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A84" t="s">
         <v>91</v>
       </c>
@@ -5601,7 +5603,7 @@
         <v>760</v>
       </c>
     </row>
-    <row r="85" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A85" t="s">
         <v>92</v>
       </c>
@@ -5621,16 +5623,16 @@
         <v>772</v>
       </c>
       <c r="G85" t="s">
-        <v>817</v>
+        <v>816</v>
       </c>
       <c r="H85" t="s">
-        <v>817</v>
+        <v>816</v>
       </c>
       <c r="I85" t="s">
-        <v>891</v>
-      </c>
-    </row>
-    <row r="86" spans="1:9" x14ac:dyDescent="0.25">
+        <v>888</v>
+      </c>
+    </row>
+    <row r="86" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A86" t="s">
         <v>93</v>
       </c>
@@ -5659,7 +5661,7 @@
         <v>760</v>
       </c>
     </row>
-    <row r="87" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A87" t="s">
         <v>94</v>
       </c>
@@ -5688,7 +5690,7 @@
         <v>760</v>
       </c>
     </row>
-    <row r="88" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A88" t="s">
         <v>95</v>
       </c>
@@ -5717,7 +5719,7 @@
         <v>760</v>
       </c>
     </row>
-    <row r="89" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A89" t="s">
         <v>96</v>
       </c>
@@ -5746,7 +5748,7 @@
         <v>760</v>
       </c>
     </row>
-    <row r="90" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A90" t="s">
         <v>97</v>
       </c>
@@ -5775,7 +5777,7 @@
         <v>760</v>
       </c>
     </row>
-    <row r="91" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A91" t="s">
         <v>98</v>
       </c>
@@ -5804,7 +5806,7 @@
         <v>760</v>
       </c>
     </row>
-    <row r="92" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A92" t="s">
         <v>99</v>
       </c>
@@ -5824,16 +5826,16 @@
         <v>773</v>
       </c>
       <c r="G92" t="s">
-        <v>818</v>
+        <v>817</v>
       </c>
       <c r="H92" t="s">
-        <v>858</v>
+        <v>856</v>
       </c>
       <c r="I92" t="s">
-        <v>894</v>
-      </c>
-    </row>
-    <row r="93" spans="1:9" x14ac:dyDescent="0.25">
+        <v>891</v>
+      </c>
+    </row>
+    <row r="93" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A93" t="s">
         <v>100</v>
       </c>
@@ -5862,7 +5864,7 @@
         <v>760</v>
       </c>
     </row>
-    <row r="94" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A94" t="s">
         <v>101</v>
       </c>
@@ -5891,7 +5893,7 @@
         <v>760</v>
       </c>
     </row>
-    <row r="95" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A95" t="s">
         <v>102</v>
       </c>
@@ -5920,7 +5922,7 @@
         <v>760</v>
       </c>
     </row>
-    <row r="96" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A96" t="s">
         <v>103</v>
       </c>
@@ -5949,7 +5951,7 @@
         <v>760</v>
       </c>
     </row>
-    <row r="97" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A97" t="s">
         <v>104</v>
       </c>
@@ -5978,7 +5980,7 @@
         <v>760</v>
       </c>
     </row>
-    <row r="98" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A98" t="s">
         <v>105</v>
       </c>
@@ -6007,7 +6009,7 @@
         <v>760</v>
       </c>
     </row>
-    <row r="99" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A99" t="s">
         <v>106</v>
       </c>
@@ -6036,7 +6038,7 @@
         <v>760</v>
       </c>
     </row>
-    <row r="100" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A100" t="s">
         <v>107</v>
       </c>
@@ -6065,7 +6067,7 @@
         <v>760</v>
       </c>
     </row>
-    <row r="101" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A101" t="s">
         <v>108</v>
       </c>
@@ -6094,7 +6096,7 @@
         <v>760</v>
       </c>
     </row>
-    <row r="102" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A102" t="s">
         <v>109</v>
       </c>
@@ -6123,7 +6125,7 @@
         <v>760</v>
       </c>
     </row>
-    <row r="103" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A103" t="s">
         <v>110</v>
       </c>
@@ -6152,7 +6154,7 @@
         <v>760</v>
       </c>
     </row>
-    <row r="104" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A104" t="s">
         <v>111</v>
       </c>
@@ -6181,7 +6183,7 @@
         <v>760</v>
       </c>
     </row>
-    <row r="105" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A105" t="s">
         <v>112</v>
       </c>
@@ -6210,7 +6212,7 @@
         <v>760</v>
       </c>
     </row>
-    <row r="106" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A106" t="s">
         <v>113</v>
       </c>
@@ -6239,7 +6241,7 @@
         <v>760</v>
       </c>
     </row>
-    <row r="107" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A107" t="s">
         <v>114</v>
       </c>
@@ -6268,7 +6270,7 @@
         <v>760</v>
       </c>
     </row>
-    <row r="108" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A108" t="s">
         <v>115</v>
       </c>
@@ -6297,7 +6299,7 @@
         <v>760</v>
       </c>
     </row>
-    <row r="109" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A109" t="s">
         <v>116</v>
       </c>
@@ -6326,7 +6328,7 @@
         <v>760</v>
       </c>
     </row>
-    <row r="110" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A110" t="s">
         <v>117</v>
       </c>
@@ -6346,16 +6348,16 @@
         <v>774</v>
       </c>
       <c r="G110" t="s">
-        <v>819</v>
+        <v>818</v>
       </c>
       <c r="H110" t="s">
-        <v>819</v>
+        <v>818</v>
       </c>
       <c r="I110" t="s">
-        <v>891</v>
-      </c>
-    </row>
-    <row r="111" spans="1:9" x14ac:dyDescent="0.25">
+        <v>888</v>
+      </c>
+    </row>
+    <row r="111" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A111" t="s">
         <v>118</v>
       </c>
@@ -6384,7 +6386,7 @@
         <v>760</v>
       </c>
     </row>
-    <row r="112" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A112" t="s">
         <v>119</v>
       </c>
@@ -6413,7 +6415,7 @@
         <v>760</v>
       </c>
     </row>
-    <row r="113" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A113" t="s">
         <v>120</v>
       </c>
@@ -6442,7 +6444,7 @@
         <v>760</v>
       </c>
     </row>
-    <row r="114" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A114" t="s">
         <v>121</v>
       </c>
@@ -6471,7 +6473,7 @@
         <v>760</v>
       </c>
     </row>
-    <row r="115" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A115" t="s">
         <v>122</v>
       </c>
@@ -6500,7 +6502,7 @@
         <v>760</v>
       </c>
     </row>
-    <row r="116" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A116" t="s">
         <v>123</v>
       </c>
@@ -6529,7 +6531,7 @@
         <v>760</v>
       </c>
     </row>
-    <row r="117" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="117" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A117" t="s">
         <v>124</v>
       </c>
@@ -6558,7 +6560,7 @@
         <v>760</v>
       </c>
     </row>
-    <row r="118" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="118" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A118" t="s">
         <v>125</v>
       </c>
@@ -6587,7 +6589,7 @@
         <v>760</v>
       </c>
     </row>
-    <row r="119" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="119" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A119" t="s">
         <v>126</v>
       </c>
@@ -6616,7 +6618,7 @@
         <v>760</v>
       </c>
     </row>
-    <row r="120" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="120" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A120" t="s">
         <v>127</v>
       </c>
@@ -6645,7 +6647,7 @@
         <v>760</v>
       </c>
     </row>
-    <row r="121" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="121" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A121" t="s">
         <v>128</v>
       </c>
@@ -6674,7 +6676,7 @@
         <v>760</v>
       </c>
     </row>
-    <row r="122" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="122" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A122" t="s">
         <v>129</v>
       </c>
@@ -6703,7 +6705,7 @@
         <v>760</v>
       </c>
     </row>
-    <row r="123" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="123" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A123" t="s">
         <v>130</v>
       </c>
@@ -6732,7 +6734,7 @@
         <v>760</v>
       </c>
     </row>
-    <row r="124" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="124" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A124" t="s">
         <v>131</v>
       </c>
@@ -6761,7 +6763,7 @@
         <v>760</v>
       </c>
     </row>
-    <row r="125" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="125" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A125" t="s">
         <v>132</v>
       </c>
@@ -6781,16 +6783,16 @@
         <v>775</v>
       </c>
       <c r="G125" t="s">
-        <v>820</v>
+        <v>819</v>
       </c>
       <c r="H125" t="s">
-        <v>820</v>
+        <v>819</v>
       </c>
       <c r="I125" t="s">
-        <v>891</v>
-      </c>
-    </row>
-    <row r="126" spans="1:9" x14ac:dyDescent="0.25">
+        <v>888</v>
+      </c>
+    </row>
+    <row r="126" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A126" t="s">
         <v>133</v>
       </c>
@@ -6819,7 +6821,7 @@
         <v>760</v>
       </c>
     </row>
-    <row r="127" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="127" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A127" t="s">
         <v>134</v>
       </c>
@@ -6848,7 +6850,7 @@
         <v>760</v>
       </c>
     </row>
-    <row r="128" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="128" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A128" t="s">
         <v>135</v>
       </c>
@@ -6877,7 +6879,7 @@
         <v>760</v>
       </c>
     </row>
-    <row r="129" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="129" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A129" t="s">
         <v>136</v>
       </c>
@@ -6906,7 +6908,7 @@
         <v>760</v>
       </c>
     </row>
-    <row r="130" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="130" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A130" t="s">
         <v>137</v>
       </c>
@@ -6935,7 +6937,7 @@
         <v>760</v>
       </c>
     </row>
-    <row r="131" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="131" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A131" t="s">
         <v>138</v>
       </c>
@@ -6964,7 +6966,7 @@
         <v>760</v>
       </c>
     </row>
-    <row r="132" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="132" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A132" t="s">
         <v>139</v>
       </c>
@@ -6984,16 +6986,16 @@
         <v>776</v>
       </c>
       <c r="G132" t="s">
-        <v>821</v>
+        <v>820</v>
       </c>
       <c r="H132" t="s">
-        <v>859</v>
+        <v>857</v>
       </c>
       <c r="I132" t="s">
-        <v>895</v>
-      </c>
-    </row>
-    <row r="133" spans="1:9" x14ac:dyDescent="0.25">
+        <v>892</v>
+      </c>
+    </row>
+    <row r="133" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A133" t="s">
         <v>140</v>
       </c>
@@ -7022,7 +7024,7 @@
         <v>760</v>
       </c>
     </row>
-    <row r="134" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="134" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A134" t="s">
         <v>141</v>
       </c>
@@ -7042,16 +7044,16 @@
         <v>777</v>
       </c>
       <c r="G134" t="s">
-        <v>822</v>
+        <v>821</v>
       </c>
       <c r="H134" t="s">
-        <v>822</v>
+        <v>821</v>
       </c>
       <c r="I134" t="s">
-        <v>891</v>
-      </c>
-    </row>
-    <row r="135" spans="1:9" x14ac:dyDescent="0.25">
+        <v>888</v>
+      </c>
+    </row>
+    <row r="135" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A135" t="s">
         <v>142</v>
       </c>
@@ -7080,7 +7082,7 @@
         <v>760</v>
       </c>
     </row>
-    <row r="136" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="136" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A136" t="s">
         <v>143</v>
       </c>
@@ -7109,7 +7111,7 @@
         <v>760</v>
       </c>
     </row>
-    <row r="137" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="137" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A137" t="s">
         <v>144</v>
       </c>
@@ -7138,7 +7140,7 @@
         <v>760</v>
       </c>
     </row>
-    <row r="138" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="138" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A138" t="s">
         <v>145</v>
       </c>
@@ -7167,7 +7169,7 @@
         <v>760</v>
       </c>
     </row>
-    <row r="139" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="139" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A139" t="s">
         <v>146</v>
       </c>
@@ -7196,7 +7198,7 @@
         <v>760</v>
       </c>
     </row>
-    <row r="140" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="140" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A140" t="s">
         <v>147</v>
       </c>
@@ -7225,7 +7227,7 @@
         <v>760</v>
       </c>
     </row>
-    <row r="141" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="141" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A141" t="s">
         <v>148</v>
       </c>
@@ -7245,16 +7247,16 @@
         <v>778</v>
       </c>
       <c r="G141" t="s">
-        <v>823</v>
+        <v>822</v>
       </c>
       <c r="H141" t="s">
-        <v>860</v>
+        <v>858</v>
       </c>
       <c r="I141" t="s">
-        <v>896</v>
-      </c>
-    </row>
-    <row r="142" spans="1:9" x14ac:dyDescent="0.25">
+        <v>893</v>
+      </c>
+    </row>
+    <row r="142" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A142" t="s">
         <v>149</v>
       </c>
@@ -7283,7 +7285,7 @@
         <v>760</v>
       </c>
     </row>
-    <row r="143" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="143" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A143" t="s">
         <v>150</v>
       </c>
@@ -7312,7 +7314,7 @@
         <v>760</v>
       </c>
     </row>
-    <row r="144" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="144" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A144" t="s">
         <v>151</v>
       </c>
@@ -7341,7 +7343,7 @@
         <v>760</v>
       </c>
     </row>
-    <row r="145" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="145" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A145" t="s">
         <v>152</v>
       </c>
@@ -7370,7 +7372,7 @@
         <v>760</v>
       </c>
     </row>
-    <row r="146" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="146" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A146" t="s">
         <v>153</v>
       </c>
@@ -7390,16 +7392,16 @@
         <v>779</v>
       </c>
       <c r="G146" t="s">
-        <v>824</v>
+        <v>823</v>
       </c>
       <c r="H146" t="s">
-        <v>861</v>
+        <v>859</v>
       </c>
       <c r="I146" t="s">
-        <v>897</v>
-      </c>
-    </row>
-    <row r="147" spans="1:9" x14ac:dyDescent="0.25">
+        <v>894</v>
+      </c>
+    </row>
+    <row r="147" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A147" t="s">
         <v>154</v>
       </c>
@@ -7428,7 +7430,7 @@
         <v>760</v>
       </c>
     </row>
-    <row r="148" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="148" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A148" t="s">
         <v>155</v>
       </c>
@@ -7457,7 +7459,7 @@
         <v>760</v>
       </c>
     </row>
-    <row r="149" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="149" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A149" t="s">
         <v>156</v>
       </c>
@@ -7486,7 +7488,7 @@
         <v>760</v>
       </c>
     </row>
-    <row r="150" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="150" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A150" t="s">
         <v>157</v>
       </c>
@@ -7515,7 +7517,7 @@
         <v>760</v>
       </c>
     </row>
-    <row r="151" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="151" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A151" t="s">
         <v>158</v>
       </c>
@@ -7544,7 +7546,7 @@
         <v>760</v>
       </c>
     </row>
-    <row r="152" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="152" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A152" t="s">
         <v>159</v>
       </c>
@@ -7573,7 +7575,7 @@
         <v>760</v>
       </c>
     </row>
-    <row r="153" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="153" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A153" t="s">
         <v>160</v>
       </c>
@@ -7602,7 +7604,7 @@
         <v>760</v>
       </c>
     </row>
-    <row r="154" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="154" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A154" t="s">
         <v>161</v>
       </c>
@@ -7631,7 +7633,7 @@
         <v>760</v>
       </c>
     </row>
-    <row r="155" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="155" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A155" t="s">
         <v>162</v>
       </c>
@@ -7660,7 +7662,7 @@
         <v>760</v>
       </c>
     </row>
-    <row r="156" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="156" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A156" t="s">
         <v>163</v>
       </c>
@@ -7689,7 +7691,7 @@
         <v>760</v>
       </c>
     </row>
-    <row r="157" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="157" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A157" t="s">
         <v>164</v>
       </c>
@@ -7718,7 +7720,7 @@
         <v>760</v>
       </c>
     </row>
-    <row r="158" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="158" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A158" t="s">
         <v>165</v>
       </c>
@@ -7747,7 +7749,7 @@
         <v>760</v>
       </c>
     </row>
-    <row r="159" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="159" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A159" t="s">
         <v>166</v>
       </c>
@@ -7776,7 +7778,7 @@
         <v>760</v>
       </c>
     </row>
-    <row r="160" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="160" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A160" t="s">
         <v>167</v>
       </c>
@@ -7805,7 +7807,7 @@
         <v>760</v>
       </c>
     </row>
-    <row r="161" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="161" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A161" t="s">
         <v>168</v>
       </c>
@@ -7834,7 +7836,7 @@
         <v>760</v>
       </c>
     </row>
-    <row r="162" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="162" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A162" t="s">
         <v>169</v>
       </c>
@@ -7863,7 +7865,7 @@
         <v>760</v>
       </c>
     </row>
-    <row r="163" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="163" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A163" t="s">
         <v>170</v>
       </c>
@@ -7892,7 +7894,7 @@
         <v>760</v>
       </c>
     </row>
-    <row r="164" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="164" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A164" t="s">
         <v>171</v>
       </c>
@@ -7921,7 +7923,7 @@
         <v>760</v>
       </c>
     </row>
-    <row r="165" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="165" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A165" t="s">
         <v>172</v>
       </c>
@@ -7950,7 +7952,7 @@
         <v>760</v>
       </c>
     </row>
-    <row r="166" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="166" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A166" t="s">
         <v>173</v>
       </c>
@@ -7979,7 +7981,7 @@
         <v>760</v>
       </c>
     </row>
-    <row r="167" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="167" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A167" t="s">
         <v>174</v>
       </c>
@@ -7999,16 +8001,16 @@
         <v>780</v>
       </c>
       <c r="G167" t="s">
-        <v>825</v>
+        <v>824</v>
       </c>
       <c r="H167" t="s">
-        <v>862</v>
+        <v>860</v>
       </c>
       <c r="I167" t="s">
-        <v>896</v>
-      </c>
-    </row>
-    <row r="168" spans="1:9" x14ac:dyDescent="0.25">
+        <v>893</v>
+      </c>
+    </row>
+    <row r="168" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A168" t="s">
         <v>175</v>
       </c>
@@ -8037,7 +8039,7 @@
         <v>760</v>
       </c>
     </row>
-    <row r="169" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="169" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A169" t="s">
         <v>176</v>
       </c>
@@ -8066,7 +8068,7 @@
         <v>760</v>
       </c>
     </row>
-    <row r="170" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="170" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A170" t="s">
         <v>177</v>
       </c>
@@ -8095,7 +8097,7 @@
         <v>760</v>
       </c>
     </row>
-    <row r="171" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="171" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A171" t="s">
         <v>178</v>
       </c>
@@ -8124,7 +8126,7 @@
         <v>760</v>
       </c>
     </row>
-    <row r="172" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="172" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A172" t="s">
         <v>179</v>
       </c>
@@ -8153,7 +8155,7 @@
         <v>760</v>
       </c>
     </row>
-    <row r="173" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="173" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A173" t="s">
         <v>180</v>
       </c>
@@ -8182,7 +8184,7 @@
         <v>760</v>
       </c>
     </row>
-    <row r="174" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="174" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A174" t="s">
         <v>181</v>
       </c>
@@ -8211,7 +8213,7 @@
         <v>760</v>
       </c>
     </row>
-    <row r="175" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="175" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A175" t="s">
         <v>182</v>
       </c>
@@ -8240,7 +8242,7 @@
         <v>760</v>
       </c>
     </row>
-    <row r="176" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="176" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A176" t="s">
         <v>183</v>
       </c>
@@ -8269,7 +8271,7 @@
         <v>760</v>
       </c>
     </row>
-    <row r="177" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="177" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A177" t="s">
         <v>184</v>
       </c>
@@ -8298,7 +8300,7 @@
         <v>760</v>
       </c>
     </row>
-    <row r="178" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="178" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A178" t="s">
         <v>185</v>
       </c>
@@ -8327,7 +8329,7 @@
         <v>760</v>
       </c>
     </row>
-    <row r="179" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="179" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A179" t="s">
         <v>186</v>
       </c>
@@ -8356,7 +8358,7 @@
         <v>760</v>
       </c>
     </row>
-    <row r="180" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="180" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A180" t="s">
         <v>187</v>
       </c>
@@ -8385,7 +8387,7 @@
         <v>760</v>
       </c>
     </row>
-    <row r="181" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="181" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A181" t="s">
         <v>188</v>
       </c>
@@ -8414,7 +8416,7 @@
         <v>760</v>
       </c>
     </row>
-    <row r="182" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="182" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A182" t="s">
         <v>189</v>
       </c>
@@ -8443,7 +8445,7 @@
         <v>760</v>
       </c>
     </row>
-    <row r="183" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="183" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A183" t="s">
         <v>190</v>
       </c>
@@ -8472,7 +8474,7 @@
         <v>760</v>
       </c>
     </row>
-    <row r="184" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="184" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A184" t="s">
         <v>191</v>
       </c>
@@ -8501,7 +8503,7 @@
         <v>760</v>
       </c>
     </row>
-    <row r="185" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="185" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A185" t="s">
         <v>192</v>
       </c>
@@ -8530,7 +8532,7 @@
         <v>760</v>
       </c>
     </row>
-    <row r="186" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="186" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A186" t="s">
         <v>193</v>
       </c>
@@ -8559,7 +8561,7 @@
         <v>760</v>
       </c>
     </row>
-    <row r="187" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="187" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A187" t="s">
         <v>194</v>
       </c>
@@ -8588,7 +8590,7 @@
         <v>760</v>
       </c>
     </row>
-    <row r="188" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="188" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A188" t="s">
         <v>195</v>
       </c>
@@ -8617,7 +8619,7 @@
         <v>760</v>
       </c>
     </row>
-    <row r="189" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="189" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A189" t="s">
         <v>196</v>
       </c>
@@ -8646,7 +8648,7 @@
         <v>760</v>
       </c>
     </row>
-    <row r="190" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="190" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A190" t="s">
         <v>197</v>
       </c>
@@ -8675,7 +8677,7 @@
         <v>760</v>
       </c>
     </row>
-    <row r="191" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="191" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A191" t="s">
         <v>198</v>
       </c>
@@ -8704,7 +8706,7 @@
         <v>760</v>
       </c>
     </row>
-    <row r="192" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="192" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A192" t="s">
         <v>199</v>
       </c>
@@ -8733,7 +8735,7 @@
         <v>760</v>
       </c>
     </row>
-    <row r="193" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="193" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A193" t="s">
         <v>200</v>
       </c>
@@ -8762,7 +8764,7 @@
         <v>760</v>
       </c>
     </row>
-    <row r="194" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="194" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A194" t="s">
         <v>201</v>
       </c>
@@ -8791,7 +8793,7 @@
         <v>760</v>
       </c>
     </row>
-    <row r="195" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="195" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A195" t="s">
         <v>202</v>
       </c>
@@ -8820,7 +8822,7 @@
         <v>760</v>
       </c>
     </row>
-    <row r="196" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="196" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A196" t="s">
         <v>203</v>
       </c>
@@ -8849,7 +8851,7 @@
         <v>760</v>
       </c>
     </row>
-    <row r="197" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="197" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A197" t="s">
         <v>204</v>
       </c>
@@ -8878,7 +8880,7 @@
         <v>760</v>
       </c>
     </row>
-    <row r="198" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="198" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A198" t="s">
         <v>205</v>
       </c>
@@ -8907,7 +8909,7 @@
         <v>760</v>
       </c>
     </row>
-    <row r="199" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="199" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A199" t="s">
         <v>206</v>
       </c>
@@ -8936,7 +8938,7 @@
         <v>760</v>
       </c>
     </row>
-    <row r="200" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="200" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A200" t="s">
         <v>207</v>
       </c>
@@ -8965,7 +8967,7 @@
         <v>760</v>
       </c>
     </row>
-    <row r="201" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="201" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A201" t="s">
         <v>208</v>
       </c>
@@ -8994,7 +8996,7 @@
         <v>760</v>
       </c>
     </row>
-    <row r="202" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="202" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A202" t="s">
         <v>209</v>
       </c>
@@ -9023,7 +9025,7 @@
         <v>760</v>
       </c>
     </row>
-    <row r="203" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="203" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A203" t="s">
         <v>210</v>
       </c>
@@ -9052,7 +9054,7 @@
         <v>760</v>
       </c>
     </row>
-    <row r="204" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="204" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A204" t="s">
         <v>211</v>
       </c>
@@ -9081,7 +9083,7 @@
         <v>760</v>
       </c>
     </row>
-    <row r="205" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="205" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A205" t="s">
         <v>212</v>
       </c>
@@ -9101,16 +9103,16 @@
         <v>781</v>
       </c>
       <c r="G205" t="s">
-        <v>826</v>
+        <v>825</v>
       </c>
       <c r="H205" t="s">
-        <v>863</v>
+        <v>861</v>
       </c>
       <c r="I205" t="s">
-        <v>898</v>
-      </c>
-    </row>
-    <row r="206" spans="1:9" x14ac:dyDescent="0.25">
+        <v>895</v>
+      </c>
+    </row>
+    <row r="206" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A206" t="s">
         <v>213</v>
       </c>
@@ -9139,7 +9141,7 @@
         <v>760</v>
       </c>
     </row>
-    <row r="207" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="207" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A207" t="s">
         <v>214</v>
       </c>
@@ -9168,7 +9170,7 @@
         <v>760</v>
       </c>
     </row>
-    <row r="208" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="208" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A208" t="s">
         <v>215</v>
       </c>
@@ -9197,7 +9199,7 @@
         <v>760</v>
       </c>
     </row>
-    <row r="209" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="209" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A209" t="s">
         <v>216</v>
       </c>
@@ -9226,7 +9228,7 @@
         <v>760</v>
       </c>
     </row>
-    <row r="210" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="210" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A210" t="s">
         <v>217</v>
       </c>
@@ -9255,7 +9257,7 @@
         <v>760</v>
       </c>
     </row>
-    <row r="211" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="211" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A211" t="s">
         <v>218</v>
       </c>
@@ -9284,7 +9286,7 @@
         <v>760</v>
       </c>
     </row>
-    <row r="212" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="212" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A212" t="s">
         <v>219</v>
       </c>
@@ -9313,7 +9315,7 @@
         <v>760</v>
       </c>
     </row>
-    <row r="213" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="213" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A213" t="s">
         <v>220</v>
       </c>
@@ -9342,7 +9344,7 @@
         <v>760</v>
       </c>
     </row>
-    <row r="214" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="214" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A214" t="s">
         <v>221</v>
       </c>
@@ -9371,7 +9373,7 @@
         <v>760</v>
       </c>
     </row>
-    <row r="215" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="215" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A215" t="s">
         <v>222</v>
       </c>
@@ -9391,16 +9393,16 @@
         <v>782</v>
       </c>
       <c r="G215" t="s">
-        <v>827</v>
+        <v>826</v>
       </c>
       <c r="H215" t="s">
-        <v>864</v>
+        <v>862</v>
       </c>
       <c r="I215" t="s">
-        <v>899</v>
-      </c>
-    </row>
-    <row r="216" spans="1:9" x14ac:dyDescent="0.25">
+        <v>896</v>
+      </c>
+    </row>
+    <row r="216" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A216" t="s">
         <v>223</v>
       </c>
@@ -9429,7 +9431,7 @@
         <v>760</v>
       </c>
     </row>
-    <row r="217" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="217" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A217" t="s">
         <v>224</v>
       </c>
@@ -9458,7 +9460,7 @@
         <v>760</v>
       </c>
     </row>
-    <row r="218" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="218" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A218" t="s">
         <v>225</v>
       </c>
@@ -9487,7 +9489,7 @@
         <v>760</v>
       </c>
     </row>
-    <row r="219" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="219" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A219" t="s">
         <v>226</v>
       </c>
@@ -9516,7 +9518,7 @@
         <v>760</v>
       </c>
     </row>
-    <row r="220" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="220" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A220" t="s">
         <v>227</v>
       </c>
@@ -9545,7 +9547,7 @@
         <v>760</v>
       </c>
     </row>
-    <row r="221" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="221" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A221" t="s">
         <v>228</v>
       </c>
@@ -9574,7 +9576,7 @@
         <v>760</v>
       </c>
     </row>
-    <row r="222" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="222" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A222" t="s">
         <v>229</v>
       </c>
@@ -9603,7 +9605,7 @@
         <v>760</v>
       </c>
     </row>
-    <row r="223" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="223" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A223" t="s">
         <v>230</v>
       </c>
@@ -9632,7 +9634,7 @@
         <v>760</v>
       </c>
     </row>
-    <row r="224" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="224" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A224" t="s">
         <v>231</v>
       </c>
@@ -9661,7 +9663,7 @@
         <v>760</v>
       </c>
     </row>
-    <row r="225" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="225" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A225" t="s">
         <v>232</v>
       </c>
@@ -9681,16 +9683,16 @@
         <v>783</v>
       </c>
       <c r="G225" t="s">
-        <v>828</v>
+        <v>827</v>
       </c>
       <c r="H225" t="s">
-        <v>865</v>
+        <v>863</v>
       </c>
       <c r="I225" t="s">
-        <v>900</v>
-      </c>
-    </row>
-    <row r="226" spans="1:9" x14ac:dyDescent="0.25">
+        <v>897</v>
+      </c>
+    </row>
+    <row r="226" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A226" t="s">
         <v>233</v>
       </c>
@@ -9719,7 +9721,7 @@
         <v>760</v>
       </c>
     </row>
-    <row r="227" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="227" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A227" t="s">
         <v>234</v>
       </c>
@@ -9748,7 +9750,7 @@
         <v>760</v>
       </c>
     </row>
-    <row r="228" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="228" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A228" t="s">
         <v>235</v>
       </c>
@@ -9777,7 +9779,7 @@
         <v>760</v>
       </c>
     </row>
-    <row r="229" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="229" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A229" t="s">
         <v>236</v>
       </c>
@@ -9806,7 +9808,7 @@
         <v>760</v>
       </c>
     </row>
-    <row r="230" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="230" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A230" t="s">
         <v>237</v>
       </c>
@@ -9835,7 +9837,7 @@
         <v>760</v>
       </c>
     </row>
-    <row r="231" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="231" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A231" t="s">
         <v>238</v>
       </c>
@@ -9864,7 +9866,7 @@
         <v>760</v>
       </c>
     </row>
-    <row r="232" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="232" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A232" t="s">
         <v>239</v>
       </c>
@@ -9893,7 +9895,7 @@
         <v>760</v>
       </c>
     </row>
-    <row r="233" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="233" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A233" t="s">
         <v>240</v>
       </c>
@@ -9922,7 +9924,7 @@
         <v>760</v>
       </c>
     </row>
-    <row r="234" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="234" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A234" t="s">
         <v>241</v>
       </c>
@@ -9951,7 +9953,7 @@
         <v>760</v>
       </c>
     </row>
-    <row r="235" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="235" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A235" t="s">
         <v>242</v>
       </c>
@@ -9980,7 +9982,7 @@
         <v>760</v>
       </c>
     </row>
-    <row r="236" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="236" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A236" t="s">
         <v>243</v>
       </c>
@@ -10009,7 +10011,7 @@
         <v>760</v>
       </c>
     </row>
-    <row r="237" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="237" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A237" t="s">
         <v>244</v>
       </c>
@@ -10029,16 +10031,16 @@
         <v>784</v>
       </c>
       <c r="G237" t="s">
-        <v>829</v>
+        <v>828</v>
       </c>
       <c r="H237" t="s">
-        <v>829</v>
+        <v>828</v>
       </c>
       <c r="I237" t="s">
-        <v>891</v>
-      </c>
-    </row>
-    <row r="238" spans="1:9" x14ac:dyDescent="0.25">
+        <v>888</v>
+      </c>
+    </row>
+    <row r="238" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A238" t="s">
         <v>245</v>
       </c>
@@ -10067,7 +10069,7 @@
         <v>760</v>
       </c>
     </row>
-    <row r="239" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="239" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A239" t="s">
         <v>246</v>
       </c>
@@ -10096,7 +10098,7 @@
         <v>760</v>
       </c>
     </row>
-    <row r="240" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="240" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A240" t="s">
         <v>247</v>
       </c>
@@ -10125,7 +10127,7 @@
         <v>760</v>
       </c>
     </row>
-    <row r="241" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="241" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A241" t="s">
         <v>248</v>
       </c>
@@ -10154,7 +10156,7 @@
         <v>760</v>
       </c>
     </row>
-    <row r="242" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="242" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A242" t="s">
         <v>249</v>
       </c>
@@ -10183,7 +10185,7 @@
         <v>760</v>
       </c>
     </row>
-    <row r="243" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="243" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A243" t="s">
         <v>250</v>
       </c>
@@ -10212,7 +10214,7 @@
         <v>760</v>
       </c>
     </row>
-    <row r="244" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="244" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A244" t="s">
         <v>251</v>
       </c>
@@ -10241,7 +10243,7 @@
         <v>760</v>
       </c>
     </row>
-    <row r="245" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="245" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A245" t="s">
         <v>252</v>
       </c>
@@ -10270,7 +10272,7 @@
         <v>760</v>
       </c>
     </row>
-    <row r="246" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="246" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A246" t="s">
         <v>253</v>
       </c>
@@ -10299,7 +10301,7 @@
         <v>760</v>
       </c>
     </row>
-    <row r="247" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="247" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A247" t="s">
         <v>254</v>
       </c>
@@ -10319,16 +10321,16 @@
         <v>785</v>
       </c>
       <c r="G247" t="s">
-        <v>830</v>
+        <v>829</v>
       </c>
       <c r="H247" t="s">
-        <v>866</v>
+        <v>864</v>
       </c>
       <c r="I247" t="s">
-        <v>901</v>
-      </c>
-    </row>
-    <row r="248" spans="1:9" x14ac:dyDescent="0.25">
+        <v>898</v>
+      </c>
+    </row>
+    <row r="248" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A248" t="s">
         <v>255</v>
       </c>
@@ -10357,7 +10359,7 @@
         <v>760</v>
       </c>
     </row>
-    <row r="249" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="249" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A249" t="s">
         <v>256</v>
       </c>
@@ -10386,7 +10388,7 @@
         <v>760</v>
       </c>
     </row>
-    <row r="250" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="250" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A250" t="s">
         <v>257</v>
       </c>
@@ -10415,7 +10417,7 @@
         <v>760</v>
       </c>
     </row>
-    <row r="251" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="251" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A251" t="s">
         <v>258</v>
       </c>
@@ -10435,16 +10437,16 @@
         <v>786</v>
       </c>
       <c r="G251" t="s">
-        <v>831</v>
+        <v>830</v>
       </c>
       <c r="H251" t="s">
-        <v>831</v>
+        <v>830</v>
       </c>
       <c r="I251" t="s">
-        <v>891</v>
-      </c>
-    </row>
-    <row r="252" spans="1:9" x14ac:dyDescent="0.25">
+        <v>888</v>
+      </c>
+    </row>
+    <row r="252" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A252" t="s">
         <v>259</v>
       </c>
@@ -10473,7 +10475,7 @@
         <v>760</v>
       </c>
     </row>
-    <row r="253" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="253" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A253" t="s">
         <v>260</v>
       </c>
@@ -10502,7 +10504,7 @@
         <v>760</v>
       </c>
     </row>
-    <row r="254" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="254" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A254" t="s">
         <v>261</v>
       </c>
@@ -10531,7 +10533,7 @@
         <v>760</v>
       </c>
     </row>
-    <row r="255" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="255" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A255" t="s">
         <v>262</v>
       </c>
@@ -10560,7 +10562,7 @@
         <v>760</v>
       </c>
     </row>
-    <row r="256" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="256" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A256" t="s">
         <v>263</v>
       </c>
@@ -10589,7 +10591,7 @@
         <v>760</v>
       </c>
     </row>
-    <row r="257" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="257" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A257" t="s">
         <v>264</v>
       </c>
@@ -10618,7 +10620,7 @@
         <v>760</v>
       </c>
     </row>
-    <row r="258" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="258" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A258" t="s">
         <v>265</v>
       </c>
@@ -10647,7 +10649,7 @@
         <v>760</v>
       </c>
     </row>
-    <row r="259" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="259" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A259" t="s">
         <v>266</v>
       </c>
@@ -10676,7 +10678,7 @@
         <v>760</v>
       </c>
     </row>
-    <row r="260" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="260" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A260" t="s">
         <v>267</v>
       </c>
@@ -10705,7 +10707,7 @@
         <v>760</v>
       </c>
     </row>
-    <row r="261" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="261" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A261" t="s">
         <v>268</v>
       </c>
@@ -10725,16 +10727,16 @@
         <v>787</v>
       </c>
       <c r="G261" t="s">
-        <v>832</v>
+        <v>831</v>
       </c>
       <c r="H261" t="s">
-        <v>832</v>
+        <v>831</v>
       </c>
       <c r="I261" t="s">
-        <v>889</v>
-      </c>
-    </row>
-    <row r="262" spans="1:9" x14ac:dyDescent="0.25">
+        <v>886</v>
+      </c>
+    </row>
+    <row r="262" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A262" t="s">
         <v>269</v>
       </c>
@@ -10763,7 +10765,7 @@
         <v>760</v>
       </c>
     </row>
-    <row r="263" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="263" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A263" t="s">
         <v>270</v>
       </c>
@@ -10792,7 +10794,7 @@
         <v>760</v>
       </c>
     </row>
-    <row r="264" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="264" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A264" t="s">
         <v>271</v>
       </c>
@@ -10812,16 +10814,16 @@
         <v>788</v>
       </c>
       <c r="G264" t="s">
-        <v>833</v>
+        <v>832</v>
       </c>
       <c r="H264" t="s">
-        <v>867</v>
+        <v>865</v>
       </c>
       <c r="I264" t="s">
-        <v>900</v>
-      </c>
-    </row>
-    <row r="265" spans="1:9" x14ac:dyDescent="0.25">
+        <v>897</v>
+      </c>
+    </row>
+    <row r="265" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A265" t="s">
         <v>272</v>
       </c>
@@ -10850,7 +10852,7 @@
         <v>760</v>
       </c>
     </row>
-    <row r="266" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="266" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A266" t="s">
         <v>273</v>
       </c>
@@ -10870,16 +10872,16 @@
         <v>789</v>
       </c>
       <c r="G266" t="s">
-        <v>834</v>
+        <v>833</v>
       </c>
       <c r="H266" t="s">
-        <v>868</v>
+        <v>866</v>
       </c>
       <c r="I266" t="s">
-        <v>902</v>
-      </c>
-    </row>
-    <row r="267" spans="1:9" x14ac:dyDescent="0.25">
+        <v>899</v>
+      </c>
+    </row>
+    <row r="267" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A267" t="s">
         <v>274</v>
       </c>
@@ -10899,16 +10901,16 @@
         <v>790</v>
       </c>
       <c r="G267" t="s">
-        <v>835</v>
+        <v>834</v>
       </c>
       <c r="H267" t="s">
-        <v>869</v>
+        <v>867</v>
       </c>
       <c r="I267" t="s">
-        <v>903</v>
-      </c>
-    </row>
-    <row r="268" spans="1:9" x14ac:dyDescent="0.25">
+        <v>900</v>
+      </c>
+    </row>
+    <row r="268" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A268" t="s">
         <v>275</v>
       </c>
@@ -10937,7 +10939,7 @@
         <v>760</v>
       </c>
     </row>
-    <row r="269" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="269" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A269" t="s">
         <v>276</v>
       </c>
@@ -10966,7 +10968,7 @@
         <v>760</v>
       </c>
     </row>
-    <row r="270" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="270" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A270" t="s">
         <v>277</v>
       </c>
@@ -10995,7 +10997,7 @@
         <v>760</v>
       </c>
     </row>
-    <row r="271" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="271" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A271" t="s">
         <v>278</v>
       </c>
@@ -11015,16 +11017,16 @@
         <v>791</v>
       </c>
       <c r="G271" t="s">
-        <v>836</v>
+        <v>835</v>
       </c>
       <c r="H271" t="s">
-        <v>870</v>
+        <v>868</v>
       </c>
       <c r="I271" t="s">
-        <v>900</v>
-      </c>
-    </row>
-    <row r="272" spans="1:9" x14ac:dyDescent="0.25">
+        <v>897</v>
+      </c>
+    </row>
+    <row r="272" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A272" t="s">
         <v>279</v>
       </c>
@@ -11053,7 +11055,7 @@
         <v>760</v>
       </c>
     </row>
-    <row r="273" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="273" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A273" t="s">
         <v>280</v>
       </c>
@@ -11082,7 +11084,7 @@
         <v>760</v>
       </c>
     </row>
-    <row r="274" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="274" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A274" t="s">
         <v>281</v>
       </c>
@@ -11111,7 +11113,7 @@
         <v>760</v>
       </c>
     </row>
-    <row r="275" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="275" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A275" t="s">
         <v>94</v>
       </c>
@@ -11140,7 +11142,7 @@
         <v>760</v>
       </c>
     </row>
-    <row r="276" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="276" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A276" t="s">
         <v>282</v>
       </c>
@@ -11169,7 +11171,7 @@
         <v>760</v>
       </c>
     </row>
-    <row r="277" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="277" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A277" t="s">
         <v>283</v>
       </c>
@@ -11198,7 +11200,7 @@
         <v>760</v>
       </c>
     </row>
-    <row r="278" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="278" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A278" t="s">
         <v>284</v>
       </c>
@@ -11227,7 +11229,7 @@
         <v>760</v>
       </c>
     </row>
-    <row r="279" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="279" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A279" t="s">
         <v>285</v>
       </c>
@@ -11256,7 +11258,7 @@
         <v>760</v>
       </c>
     </row>
-    <row r="280" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="280" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A280" t="s">
         <v>286</v>
       </c>
@@ -11285,7 +11287,7 @@
         <v>760</v>
       </c>
     </row>
-    <row r="281" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="281" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A281" t="s">
         <v>287</v>
       </c>
@@ -11314,7 +11316,7 @@
         <v>760</v>
       </c>
     </row>
-    <row r="282" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="282" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A282" t="s">
         <v>288</v>
       </c>
@@ -11343,7 +11345,7 @@
         <v>760</v>
       </c>
     </row>
-    <row r="283" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="283" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A283" t="s">
         <v>289</v>
       </c>
@@ -11372,7 +11374,7 @@
         <v>760</v>
       </c>
     </row>
-    <row r="284" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="284" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A284" t="s">
         <v>290</v>
       </c>
@@ -11392,16 +11394,16 @@
         <v>792</v>
       </c>
       <c r="G284" t="s">
-        <v>837</v>
+        <v>836</v>
       </c>
       <c r="H284" t="s">
-        <v>871</v>
+        <v>869</v>
       </c>
       <c r="I284" t="s">
-        <v>904</v>
-      </c>
-    </row>
-    <row r="285" spans="1:9" x14ac:dyDescent="0.25">
+        <v>901</v>
+      </c>
+    </row>
+    <row r="285" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A285" t="s">
         <v>291</v>
       </c>
@@ -11430,7 +11432,7 @@
         <v>760</v>
       </c>
     </row>
-    <row r="286" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="286" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A286" t="s">
         <v>292</v>
       </c>
@@ -11459,7 +11461,7 @@
         <v>760</v>
       </c>
     </row>
-    <row r="287" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="287" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A287" t="s">
         <v>293</v>
       </c>
@@ -11479,16 +11481,16 @@
         <v>793</v>
       </c>
       <c r="G287" t="s">
-        <v>838</v>
+        <v>837</v>
       </c>
       <c r="H287" t="s">
-        <v>872</v>
+        <v>870</v>
       </c>
       <c r="I287" t="s">
-        <v>905</v>
-      </c>
-    </row>
-    <row r="288" spans="1:9" x14ac:dyDescent="0.25">
+        <v>902</v>
+      </c>
+    </row>
+    <row r="288" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A288" t="s">
         <v>294</v>
       </c>
@@ -11517,7 +11519,7 @@
         <v>760</v>
       </c>
     </row>
-    <row r="289" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="289" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A289" t="s">
         <v>295</v>
       </c>
@@ -11546,7 +11548,7 @@
         <v>760</v>
       </c>
     </row>
-    <row r="290" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="290" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A290" t="s">
         <v>296</v>
       </c>
@@ -11566,16 +11568,16 @@
         <v>794</v>
       </c>
       <c r="G290" t="s">
-        <v>839</v>
+        <v>838</v>
       </c>
       <c r="H290" t="s">
-        <v>873</v>
+        <v>871</v>
       </c>
       <c r="I290" t="s">
-        <v>906</v>
-      </c>
-    </row>
-    <row r="291" spans="1:9" x14ac:dyDescent="0.25">
+        <v>903</v>
+      </c>
+    </row>
+    <row r="291" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A291" t="s">
         <v>297</v>
       </c>
@@ -11604,7 +11606,7 @@
         <v>760</v>
       </c>
     </row>
-    <row r="292" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="292" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A292" t="s">
         <v>298</v>
       </c>
@@ -11633,7 +11635,7 @@
         <v>760</v>
       </c>
     </row>
-    <row r="293" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="293" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A293" t="s">
         <v>299</v>
       </c>
@@ -11653,16 +11655,16 @@
         <v>795</v>
       </c>
       <c r="G293" t="s">
-        <v>840</v>
+        <v>839</v>
       </c>
       <c r="H293" t="s">
-        <v>874</v>
+        <v>872</v>
       </c>
       <c r="I293" t="s">
-        <v>907</v>
-      </c>
-    </row>
-    <row r="294" spans="1:9" x14ac:dyDescent="0.25">
+        <v>904</v>
+      </c>
+    </row>
+    <row r="294" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A294" t="s">
         <v>300</v>
       </c>
@@ -11691,7 +11693,7 @@
         <v>760</v>
       </c>
     </row>
-    <row r="295" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="295" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A295" t="s">
         <v>301</v>
       </c>
@@ -11720,7 +11722,7 @@
         <v>760</v>
       </c>
     </row>
-    <row r="296" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="296" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A296" t="s">
         <v>302</v>
       </c>
@@ -11749,7 +11751,7 @@
         <v>760</v>
       </c>
     </row>
-    <row r="297" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="297" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A297" t="s">
         <v>303</v>
       </c>
@@ -11766,13 +11768,13 @@
         <v>705</v>
       </c>
       <c r="F297" t="s">
-        <v>915</v>
+        <v>911</v>
       </c>
       <c r="G297" t="s">
-        <v>916</v>
-      </c>
-    </row>
-    <row r="298" spans="1:9" x14ac:dyDescent="0.25">
+        <v>912</v>
+      </c>
+    </row>
+    <row r="298" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A298" t="s">
         <v>304</v>
       </c>
@@ -11792,16 +11794,16 @@
         <v>796</v>
       </c>
       <c r="G298" t="s">
-        <v>841</v>
+        <v>840</v>
       </c>
       <c r="H298" t="s">
-        <v>875</v>
+        <v>873</v>
       </c>
       <c r="I298" t="s">
-        <v>908</v>
-      </c>
-    </row>
-    <row r="299" spans="1:9" x14ac:dyDescent="0.25">
+        <v>905</v>
+      </c>
+    </row>
+    <row r="299" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A299" t="s">
         <v>305</v>
       </c>
@@ -11821,18 +11823,18 @@
         <v>797</v>
       </c>
       <c r="G299" t="s">
-        <v>842</v>
+        <v>841</v>
       </c>
       <c r="H299" t="s">
-        <v>842</v>
+        <v>841</v>
       </c>
       <c r="I299" t="s">
-        <v>891</v>
-      </c>
-    </row>
-    <row r="300" spans="1:9" x14ac:dyDescent="0.25">
+        <v>888</v>
+      </c>
+    </row>
+    <row r="300" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A300" t="s">
-        <v>917</v>
+        <v>913</v>
       </c>
       <c r="B300" t="s">
         <v>378</v>
@@ -11847,10 +11849,10 @@
         <v>708</v>
       </c>
       <c r="F300" t="s">
-        <v>918</v>
-      </c>
-    </row>
-    <row r="301" spans="1:9" x14ac:dyDescent="0.25">
+        <v>914</v>
+      </c>
+    </row>
+    <row r="301" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A301" t="s">
         <v>306</v>
       </c>
@@ -11879,7 +11881,7 @@
         <v>760</v>
       </c>
     </row>
-    <row r="302" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="302" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A302" t="s">
         <v>307</v>
       </c>
@@ -11908,7 +11910,7 @@
         <v>760</v>
       </c>
     </row>
-    <row r="303" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="303" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A303" t="s">
         <v>308</v>
       </c>
@@ -11937,7 +11939,7 @@
         <v>760</v>
       </c>
     </row>
-    <row r="304" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="304" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A304" t="s">
         <v>309</v>
       </c>
@@ -11966,7 +11968,7 @@
         <v>760</v>
       </c>
     </row>
-    <row r="305" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="305" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A305" t="s">
         <v>310</v>
       </c>
@@ -11986,16 +11988,16 @@
         <v>798</v>
       </c>
       <c r="G305" t="s">
-        <v>843</v>
+        <v>842</v>
       </c>
       <c r="H305" t="s">
-        <v>876</v>
+        <v>874</v>
       </c>
       <c r="I305" t="s">
-        <v>909</v>
-      </c>
-    </row>
-    <row r="306" spans="1:9" x14ac:dyDescent="0.25">
+        <v>906</v>
+      </c>
+    </row>
+    <row r="306" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A306" t="s">
         <v>311</v>
       </c>
@@ -12015,16 +12017,16 @@
         <v>799</v>
       </c>
       <c r="G306" t="s">
-        <v>844</v>
+        <v>843</v>
       </c>
       <c r="H306" t="s">
-        <v>844</v>
+        <v>843</v>
       </c>
       <c r="I306" t="s">
-        <v>891</v>
-      </c>
-    </row>
-    <row r="307" spans="1:9" x14ac:dyDescent="0.25">
+        <v>888</v>
+      </c>
+    </row>
+    <row r="307" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A307" t="s">
         <v>312</v>
       </c>
@@ -12044,16 +12046,16 @@
         <v>800</v>
       </c>
       <c r="G307" t="s">
-        <v>845</v>
+        <v>844</v>
       </c>
       <c r="H307" t="s">
-        <v>877</v>
+        <v>875</v>
       </c>
       <c r="I307" t="s">
-        <v>908</v>
-      </c>
-    </row>
-    <row r="308" spans="1:9" x14ac:dyDescent="0.25">
+        <v>905</v>
+      </c>
+    </row>
+    <row r="308" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A308" t="s">
         <v>313</v>
       </c>
@@ -12070,13 +12072,13 @@
         <v>716</v>
       </c>
       <c r="F308" t="s">
-        <v>919</v>
+        <v>915</v>
       </c>
       <c r="G308" t="s">
-        <v>920</v>
-      </c>
-    </row>
-    <row r="309" spans="1:9" x14ac:dyDescent="0.25">
+        <v>916</v>
+      </c>
+    </row>
+    <row r="309" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A309" t="s">
         <v>314</v>
       </c>
@@ -12105,7 +12107,7 @@
         <v>760</v>
       </c>
     </row>
-    <row r="310" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="310" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A310" t="s">
         <v>315</v>
       </c>
@@ -12125,16 +12127,16 @@
         <v>801</v>
       </c>
       <c r="G310" t="s">
-        <v>846</v>
+        <v>845</v>
       </c>
       <c r="H310" t="s">
-        <v>846</v>
+        <v>845</v>
       </c>
       <c r="I310" t="s">
-        <v>891</v>
-      </c>
-    </row>
-    <row r="311" spans="1:9" x14ac:dyDescent="0.25">
+        <v>888</v>
+      </c>
+    </row>
+    <row r="311" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A311" t="s">
         <v>316</v>
       </c>
@@ -12154,16 +12156,16 @@
         <v>802</v>
       </c>
       <c r="G311" t="s">
-        <v>847</v>
+        <v>846</v>
       </c>
       <c r="H311" t="s">
-        <v>878</v>
+        <v>876</v>
       </c>
       <c r="I311" t="s">
-        <v>898</v>
-      </c>
-    </row>
-    <row r="312" spans="1:9" x14ac:dyDescent="0.25">
+        <v>895</v>
+      </c>
+    </row>
+    <row r="312" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A312" t="s">
         <v>317</v>
       </c>
@@ -12180,19 +12182,19 @@
         <v>720</v>
       </c>
       <c r="F312" t="s">
-        <v>803</v>
+        <v>919</v>
       </c>
       <c r="G312" t="s">
-        <v>848</v>
+        <v>917</v>
       </c>
       <c r="H312" t="s">
-        <v>879</v>
+        <v>918</v>
       </c>
       <c r="I312" t="s">
-        <v>910</v>
-      </c>
-    </row>
-    <row r="313" spans="1:9" x14ac:dyDescent="0.25">
+        <v>760</v>
+      </c>
+    </row>
+    <row r="313" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A313" t="s">
         <v>318</v>
       </c>
@@ -12221,7 +12223,7 @@
         <v>760</v>
       </c>
     </row>
-    <row r="314" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="314" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A314" t="s">
         <v>319</v>
       </c>
@@ -12238,19 +12240,19 @@
         <v>722</v>
       </c>
       <c r="F314" t="s">
-        <v>804</v>
+        <v>803</v>
       </c>
       <c r="G314" t="s">
-        <v>849</v>
+        <v>847</v>
       </c>
       <c r="H314" t="s">
-        <v>880</v>
+        <v>877</v>
       </c>
       <c r="I314" t="s">
-        <v>899</v>
-      </c>
-    </row>
-    <row r="315" spans="1:9" x14ac:dyDescent="0.25">
+        <v>896</v>
+      </c>
+    </row>
+    <row r="315" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A315" t="s">
         <v>320</v>
       </c>
@@ -12279,7 +12281,7 @@
         <v>760</v>
       </c>
     </row>
-    <row r="316" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="316" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A316" t="s">
         <v>321</v>
       </c>
@@ -12296,19 +12298,19 @@
         <v>724</v>
       </c>
       <c r="F316" t="s">
-        <v>805</v>
+        <v>804</v>
       </c>
       <c r="G316" t="s">
-        <v>850</v>
+        <v>848</v>
       </c>
       <c r="H316" t="s">
-        <v>881</v>
+        <v>878</v>
       </c>
       <c r="I316" t="s">
-        <v>911</v>
-      </c>
-    </row>
-    <row r="317" spans="1:9" x14ac:dyDescent="0.25">
+        <v>907</v>
+      </c>
+    </row>
+    <row r="317" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A317" t="s">
         <v>322</v>
       </c>
@@ -12337,7 +12339,7 @@
         <v>760</v>
       </c>
     </row>
-    <row r="318" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="318" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A318" t="s">
         <v>323</v>
       </c>
@@ -12366,7 +12368,7 @@
         <v>760</v>
       </c>
     </row>
-    <row r="319" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="319" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A319" t="s">
         <v>324</v>
       </c>
@@ -12395,7 +12397,7 @@
         <v>760</v>
       </c>
     </row>
-    <row r="320" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="320" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A320" t="s">
         <v>325</v>
       </c>
@@ -12424,7 +12426,7 @@
         <v>760</v>
       </c>
     </row>
-    <row r="321" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="321" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A321" t="s">
         <v>326</v>
       </c>
@@ -12453,7 +12455,7 @@
         <v>760</v>
       </c>
     </row>
-    <row r="322" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="322" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A322" t="s">
         <v>327</v>
       </c>
@@ -12482,7 +12484,7 @@
         <v>760</v>
       </c>
     </row>
-    <row r="323" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="323" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A323" t="s">
         <v>328</v>
       </c>
@@ -12511,7 +12513,7 @@
         <v>760</v>
       </c>
     </row>
-    <row r="324" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="324" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A324" t="s">
         <v>329</v>
       </c>
@@ -12540,7 +12542,7 @@
         <v>760</v>
       </c>
     </row>
-    <row r="325" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="325" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A325" t="s">
         <v>330</v>
       </c>
@@ -12569,7 +12571,7 @@
         <v>760</v>
       </c>
     </row>
-    <row r="326" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="326" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A326" t="s">
         <v>331</v>
       </c>
@@ -12598,7 +12600,7 @@
         <v>760</v>
       </c>
     </row>
-    <row r="327" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="327" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A327" t="s">
         <v>332</v>
       </c>
@@ -12627,7 +12629,7 @@
         <v>760</v>
       </c>
     </row>
-    <row r="328" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="328" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A328" t="s">
         <v>333</v>
       </c>
@@ -12656,7 +12658,7 @@
         <v>760</v>
       </c>
     </row>
-    <row r="329" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="329" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A329" t="s">
         <v>334</v>
       </c>
@@ -12685,7 +12687,7 @@
         <v>760</v>
       </c>
     </row>
-    <row r="330" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="330" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A330" t="s">
         <v>335</v>
       </c>
@@ -12714,7 +12716,7 @@
         <v>760</v>
       </c>
     </row>
-    <row r="331" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="331" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A331" t="s">
         <v>336</v>
       </c>
@@ -12743,7 +12745,7 @@
         <v>760</v>
       </c>
     </row>
-    <row r="332" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="332" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A332" t="s">
         <v>337</v>
       </c>
@@ -12772,7 +12774,7 @@
         <v>760</v>
       </c>
     </row>
-    <row r="333" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="333" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A333" t="s">
         <v>338</v>
       </c>
@@ -12801,7 +12803,7 @@
         <v>760</v>
       </c>
     </row>
-    <row r="334" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="334" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A334" t="s">
         <v>339</v>
       </c>
@@ -12830,7 +12832,7 @@
         <v>760</v>
       </c>
     </row>
-    <row r="335" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="335" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A335" t="s">
         <v>340</v>
       </c>
@@ -12859,7 +12861,7 @@
         <v>760</v>
       </c>
     </row>
-    <row r="336" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="336" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A336" t="s">
         <v>341</v>
       </c>
@@ -12888,7 +12890,7 @@
         <v>760</v>
       </c>
     </row>
-    <row r="337" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="337" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A337" t="s">
         <v>342</v>
       </c>
@@ -12917,7 +12919,7 @@
         <v>760</v>
       </c>
     </row>
-    <row r="338" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="338" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A338" t="s">
         <v>343</v>
       </c>
@@ -12946,7 +12948,7 @@
         <v>760</v>
       </c>
     </row>
-    <row r="339" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="339" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A339" t="s">
         <v>344</v>
       </c>
@@ -12975,7 +12977,7 @@
         <v>760</v>
       </c>
     </row>
-    <row r="340" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="340" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A340" t="s">
         <v>345</v>
       </c>
@@ -13004,7 +13006,7 @@
         <v>760</v>
       </c>
     </row>
-    <row r="341" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="341" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A341" t="s">
         <v>346</v>
       </c>
@@ -13033,7 +13035,7 @@
         <v>760</v>
       </c>
     </row>
-    <row r="342" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="342" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A342" t="s">
         <v>347</v>
       </c>
@@ -13062,7 +13064,7 @@
         <v>760</v>
       </c>
     </row>
-    <row r="343" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="343" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A343" t="s">
         <v>348</v>
       </c>
@@ -13091,7 +13093,7 @@
         <v>760</v>
       </c>
     </row>
-    <row r="344" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="344" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A344" t="s">
         <v>349</v>
       </c>
@@ -13120,7 +13122,7 @@
         <v>760</v>
       </c>
     </row>
-    <row r="345" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="345" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A345" t="s">
         <v>350</v>
       </c>
@@ -13149,7 +13151,7 @@
         <v>760</v>
       </c>
     </row>
-    <row r="346" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="346" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A346" t="s">
         <v>351</v>
       </c>
@@ -13178,7 +13180,7 @@
         <v>760</v>
       </c>
     </row>
-    <row r="347" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="347" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A347" t="s">
         <v>352</v>
       </c>
@@ -13207,7 +13209,7 @@
         <v>760</v>
       </c>
     </row>
-    <row r="348" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="348" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A348" t="s">
         <v>353</v>
       </c>
@@ -13236,7 +13238,7 @@
         <v>760</v>
       </c>
     </row>
-    <row r="349" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="349" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A349" t="s">
         <v>354</v>
       </c>
@@ -13265,7 +13267,7 @@
         <v>760</v>
       </c>
     </row>
-    <row r="350" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="350" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A350" t="s">
         <v>355</v>
       </c>
@@ -13294,7 +13296,7 @@
         <v>760</v>
       </c>
     </row>
-    <row r="351" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="351" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A351" t="s">
         <v>356</v>
       </c>

</xml_diff>

<commit_message>
adding sortlistet as columns
</commit_message>
<xml_diff>
--- a/data/Eksklusionslister/PenSam_eksklusionsliste_isin.xlsx
+++ b/data/Eksklusionslister/PenSam_eksklusionsliste_isin.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Anja\OneDrive - Gravercentret\Dokumenter\Python_projekter\kommune_investering\data\Eksklusionslister\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E0F46520-6EA2-468E-91DC-C5B573A57013}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{274359F5-2FB8-4601-BC73-533B143A0A6C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -3156,18 +3156,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:I351"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A298" workbookViewId="0">
-      <selection activeCell="F310" sqref="F310"/>
+    <sheetView tabSelected="1" topLeftCell="C298" workbookViewId="0">
+      <selection activeCell="F312" sqref="F312"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="54" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="162.77734375" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="200.88671875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="162.7109375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="200.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -3196,7 +3196,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>9</v>
       </c>
@@ -3225,7 +3225,7 @@
         <v>760</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>10</v>
       </c>
@@ -3254,7 +3254,7 @@
         <v>760</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>11</v>
       </c>
@@ -3283,7 +3283,7 @@
         <v>879</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>12</v>
       </c>
@@ -3312,7 +3312,7 @@
         <v>760</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>13</v>
       </c>
@@ -3341,7 +3341,7 @@
         <v>760</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>14</v>
       </c>
@@ -3370,7 +3370,7 @@
         <v>760</v>
       </c>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>15</v>
       </c>
@@ -3399,7 +3399,7 @@
         <v>760</v>
       </c>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>16</v>
       </c>
@@ -3428,7 +3428,7 @@
         <v>880</v>
       </c>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>17</v>
       </c>
@@ -3457,7 +3457,7 @@
         <v>881</v>
       </c>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
         <v>18</v>
       </c>
@@ -3486,7 +3486,7 @@
         <v>882</v>
       </c>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>19</v>
       </c>
@@ -3515,7 +3515,7 @@
         <v>760</v>
       </c>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>20</v>
       </c>
@@ -3544,7 +3544,7 @@
         <v>883</v>
       </c>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>21</v>
       </c>
@@ -3573,7 +3573,7 @@
         <v>884</v>
       </c>
     </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>22</v>
       </c>
@@ -3602,7 +3602,7 @@
         <v>760</v>
       </c>
     </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>23</v>
       </c>
@@ -3631,7 +3631,7 @@
         <v>760</v>
       </c>
     </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>24</v>
       </c>
@@ -3660,7 +3660,7 @@
         <v>760</v>
       </c>
     </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>25</v>
       </c>
@@ -3689,7 +3689,7 @@
         <v>760</v>
       </c>
     </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>26</v>
       </c>
@@ -3718,7 +3718,7 @@
         <v>760</v>
       </c>
     </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>27</v>
       </c>
@@ -3747,7 +3747,7 @@
         <v>760</v>
       </c>
     </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>28</v>
       </c>
@@ -3776,7 +3776,7 @@
         <v>760</v>
       </c>
     </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>29</v>
       </c>
@@ -3805,7 +3805,7 @@
         <v>760</v>
       </c>
     </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>30</v>
       </c>
@@ -3834,7 +3834,7 @@
         <v>760</v>
       </c>
     </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>31</v>
       </c>
@@ -3863,7 +3863,7 @@
         <v>760</v>
       </c>
     </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>32</v>
       </c>
@@ -3892,7 +3892,7 @@
         <v>760</v>
       </c>
     </row>
-    <row r="26" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>33</v>
       </c>
@@ -3921,7 +3921,7 @@
         <v>885</v>
       </c>
     </row>
-    <row r="27" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>34</v>
       </c>
@@ -3950,7 +3950,7 @@
         <v>760</v>
       </c>
     </row>
-    <row r="28" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>35</v>
       </c>
@@ -3979,7 +3979,7 @@
         <v>760</v>
       </c>
     </row>
-    <row r="29" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>36</v>
       </c>
@@ -4008,7 +4008,7 @@
         <v>760</v>
       </c>
     </row>
-    <row r="30" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>37</v>
       </c>
@@ -4037,7 +4037,7 @@
         <v>760</v>
       </c>
     </row>
-    <row r="31" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>38</v>
       </c>
@@ -4066,7 +4066,7 @@
         <v>760</v>
       </c>
     </row>
-    <row r="32" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>39</v>
       </c>
@@ -4095,7 +4095,7 @@
         <v>886</v>
       </c>
     </row>
-    <row r="33" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>40</v>
       </c>
@@ -4124,7 +4124,7 @@
         <v>760</v>
       </c>
     </row>
-    <row r="34" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>41</v>
       </c>
@@ -4153,7 +4153,7 @@
         <v>760</v>
       </c>
     </row>
-    <row r="35" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>42</v>
       </c>
@@ -4182,7 +4182,7 @@
         <v>760</v>
       </c>
     </row>
-    <row r="36" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>43</v>
       </c>
@@ -4211,7 +4211,7 @@
         <v>760</v>
       </c>
     </row>
-    <row r="37" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>44</v>
       </c>
@@ -4240,7 +4240,7 @@
         <v>760</v>
       </c>
     </row>
-    <row r="38" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>45</v>
       </c>
@@ -4269,7 +4269,7 @@
         <v>760</v>
       </c>
     </row>
-    <row r="39" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>46</v>
       </c>
@@ -4298,7 +4298,7 @@
         <v>760</v>
       </c>
     </row>
-    <row r="40" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>47</v>
       </c>
@@ -4327,7 +4327,7 @@
         <v>760</v>
       </c>
     </row>
-    <row r="41" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
         <v>48</v>
       </c>
@@ -4356,7 +4356,7 @@
         <v>887</v>
       </c>
     </row>
-    <row r="42" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
         <v>49</v>
       </c>
@@ -4385,7 +4385,7 @@
         <v>760</v>
       </c>
     </row>
-    <row r="43" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
         <v>50</v>
       </c>
@@ -4414,7 +4414,7 @@
         <v>760</v>
       </c>
     </row>
-    <row r="44" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
         <v>51</v>
       </c>
@@ -4443,7 +4443,7 @@
         <v>760</v>
       </c>
     </row>
-    <row r="45" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
         <v>52</v>
       </c>
@@ -4472,7 +4472,7 @@
         <v>760</v>
       </c>
     </row>
-    <row r="46" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
         <v>53</v>
       </c>
@@ -4501,7 +4501,7 @@
         <v>760</v>
       </c>
     </row>
-    <row r="47" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
         <v>54</v>
       </c>
@@ -4530,7 +4530,7 @@
         <v>760</v>
       </c>
     </row>
-    <row r="48" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
         <v>55</v>
       </c>
@@ -4559,7 +4559,7 @@
         <v>760</v>
       </c>
     </row>
-    <row r="49" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
         <v>56</v>
       </c>
@@ -4588,7 +4588,7 @@
         <v>760</v>
       </c>
     </row>
-    <row r="50" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
         <v>57</v>
       </c>
@@ -4617,7 +4617,7 @@
         <v>760</v>
       </c>
     </row>
-    <row r="51" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
         <v>58</v>
       </c>
@@ -4646,7 +4646,7 @@
         <v>760</v>
       </c>
     </row>
-    <row r="52" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
         <v>59</v>
       </c>
@@ -4675,7 +4675,7 @@
         <v>888</v>
       </c>
     </row>
-    <row r="53" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
         <v>60</v>
       </c>
@@ -4704,7 +4704,7 @@
         <v>889</v>
       </c>
     </row>
-    <row r="54" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
         <v>61</v>
       </c>
@@ -4733,7 +4733,7 @@
         <v>760</v>
       </c>
     </row>
-    <row r="55" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
         <v>62</v>
       </c>
@@ -4762,7 +4762,7 @@
         <v>890</v>
       </c>
     </row>
-    <row r="56" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
         <v>63</v>
       </c>
@@ -4791,7 +4791,7 @@
         <v>760</v>
       </c>
     </row>
-    <row r="57" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
         <v>64</v>
       </c>
@@ -4820,7 +4820,7 @@
         <v>760</v>
       </c>
     </row>
-    <row r="58" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
         <v>65</v>
       </c>
@@ -4849,7 +4849,7 @@
         <v>760</v>
       </c>
     </row>
-    <row r="59" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
         <v>66</v>
       </c>
@@ -4878,7 +4878,7 @@
         <v>760</v>
       </c>
     </row>
-    <row r="60" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
         <v>67</v>
       </c>
@@ -4907,7 +4907,7 @@
         <v>760</v>
       </c>
     </row>
-    <row r="61" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
         <v>68</v>
       </c>
@@ -4936,7 +4936,7 @@
         <v>760</v>
       </c>
     </row>
-    <row r="62" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
         <v>69</v>
       </c>
@@ -4965,7 +4965,7 @@
         <v>760</v>
       </c>
     </row>
-    <row r="63" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
         <v>70</v>
       </c>
@@ -4994,7 +4994,7 @@
         <v>760</v>
       </c>
     </row>
-    <row r="64" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
         <v>71</v>
       </c>
@@ -5023,7 +5023,7 @@
         <v>760</v>
       </c>
     </row>
-    <row r="65" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
         <v>72</v>
       </c>
@@ -5052,7 +5052,7 @@
         <v>760</v>
       </c>
     </row>
-    <row r="66" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
         <v>73</v>
       </c>
@@ -5081,7 +5081,7 @@
         <v>760</v>
       </c>
     </row>
-    <row r="67" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
         <v>74</v>
       </c>
@@ -5110,7 +5110,7 @@
         <v>760</v>
       </c>
     </row>
-    <row r="68" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
         <v>75</v>
       </c>
@@ -5139,7 +5139,7 @@
         <v>760</v>
       </c>
     </row>
-    <row r="69" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
         <v>76</v>
       </c>
@@ -5168,7 +5168,7 @@
         <v>760</v>
       </c>
     </row>
-    <row r="70" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
         <v>77</v>
       </c>
@@ -5197,7 +5197,7 @@
         <v>760</v>
       </c>
     </row>
-    <row r="71" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
         <v>78</v>
       </c>
@@ -5226,7 +5226,7 @@
         <v>760</v>
       </c>
     </row>
-    <row r="72" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="72" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
         <v>79</v>
       </c>
@@ -5255,7 +5255,7 @@
         <v>760</v>
       </c>
     </row>
-    <row r="73" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="73" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
         <v>80</v>
       </c>
@@ -5284,7 +5284,7 @@
         <v>760</v>
       </c>
     </row>
-    <row r="74" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="74" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
         <v>81</v>
       </c>
@@ -5313,7 +5313,7 @@
         <v>760</v>
       </c>
     </row>
-    <row r="75" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="75" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
         <v>82</v>
       </c>
@@ -5342,7 +5342,7 @@
         <v>760</v>
       </c>
     </row>
-    <row r="76" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="76" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
         <v>83</v>
       </c>
@@ -5371,7 +5371,7 @@
         <v>760</v>
       </c>
     </row>
-    <row r="77" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="77" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
         <v>84</v>
       </c>
@@ -5400,7 +5400,7 @@
         <v>760</v>
       </c>
     </row>
-    <row r="78" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="78" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
         <v>85</v>
       </c>
@@ -5429,7 +5429,7 @@
         <v>760</v>
       </c>
     </row>
-    <row r="79" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="79" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
         <v>86</v>
       </c>
@@ -5458,7 +5458,7 @@
         <v>760</v>
       </c>
     </row>
-    <row r="80" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="80" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
         <v>87</v>
       </c>
@@ -5487,7 +5487,7 @@
         <v>760</v>
       </c>
     </row>
-    <row r="81" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="81" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A81" t="s">
         <v>88</v>
       </c>
@@ -5516,7 +5516,7 @@
         <v>760</v>
       </c>
     </row>
-    <row r="82" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="82" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A82" t="s">
         <v>89</v>
       </c>
@@ -5545,7 +5545,7 @@
         <v>760</v>
       </c>
     </row>
-    <row r="83" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="83" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A83" t="s">
         <v>90</v>
       </c>
@@ -5574,7 +5574,7 @@
         <v>760</v>
       </c>
     </row>
-    <row r="84" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="84" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A84" t="s">
         <v>91</v>
       </c>
@@ -5603,7 +5603,7 @@
         <v>760</v>
       </c>
     </row>
-    <row r="85" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="85" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A85" t="s">
         <v>92</v>
       </c>
@@ -5632,7 +5632,7 @@
         <v>888</v>
       </c>
     </row>
-    <row r="86" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="86" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A86" t="s">
         <v>93</v>
       </c>
@@ -5661,7 +5661,7 @@
         <v>760</v>
       </c>
     </row>
-    <row r="87" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="87" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A87" t="s">
         <v>94</v>
       </c>
@@ -5690,7 +5690,7 @@
         <v>760</v>
       </c>
     </row>
-    <row r="88" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="88" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A88" t="s">
         <v>95</v>
       </c>
@@ -5719,7 +5719,7 @@
         <v>760</v>
       </c>
     </row>
-    <row r="89" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="89" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A89" t="s">
         <v>96</v>
       </c>
@@ -5748,7 +5748,7 @@
         <v>760</v>
       </c>
     </row>
-    <row r="90" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="90" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A90" t="s">
         <v>97</v>
       </c>
@@ -5777,7 +5777,7 @@
         <v>760</v>
       </c>
     </row>
-    <row r="91" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="91" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A91" t="s">
         <v>98</v>
       </c>
@@ -5806,7 +5806,7 @@
         <v>760</v>
       </c>
     </row>
-    <row r="92" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="92" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A92" t="s">
         <v>99</v>
       </c>
@@ -5835,7 +5835,7 @@
         <v>891</v>
       </c>
     </row>
-    <row r="93" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="93" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A93" t="s">
         <v>100</v>
       </c>
@@ -5864,7 +5864,7 @@
         <v>760</v>
       </c>
     </row>
-    <row r="94" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="94" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A94" t="s">
         <v>101</v>
       </c>
@@ -5893,7 +5893,7 @@
         <v>760</v>
       </c>
     </row>
-    <row r="95" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="95" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A95" t="s">
         <v>102</v>
       </c>
@@ -5922,7 +5922,7 @@
         <v>760</v>
       </c>
     </row>
-    <row r="96" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="96" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A96" t="s">
         <v>103</v>
       </c>
@@ -5951,7 +5951,7 @@
         <v>760</v>
       </c>
     </row>
-    <row r="97" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="97" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A97" t="s">
         <v>104</v>
       </c>
@@ -5980,7 +5980,7 @@
         <v>760</v>
       </c>
     </row>
-    <row r="98" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="98" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A98" t="s">
         <v>105</v>
       </c>
@@ -6009,7 +6009,7 @@
         <v>760</v>
       </c>
     </row>
-    <row r="99" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="99" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A99" t="s">
         <v>106</v>
       </c>
@@ -6038,7 +6038,7 @@
         <v>760</v>
       </c>
     </row>
-    <row r="100" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="100" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A100" t="s">
         <v>107</v>
       </c>
@@ -6067,7 +6067,7 @@
         <v>760</v>
       </c>
     </row>
-    <row r="101" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="101" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A101" t="s">
         <v>108</v>
       </c>
@@ -6096,7 +6096,7 @@
         <v>760</v>
       </c>
     </row>
-    <row r="102" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="102" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A102" t="s">
         <v>109</v>
       </c>
@@ -6125,7 +6125,7 @@
         <v>760</v>
       </c>
     </row>
-    <row r="103" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="103" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A103" t="s">
         <v>110</v>
       </c>
@@ -6154,7 +6154,7 @@
         <v>760</v>
       </c>
     </row>
-    <row r="104" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="104" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A104" t="s">
         <v>111</v>
       </c>
@@ -6183,7 +6183,7 @@
         <v>760</v>
       </c>
     </row>
-    <row r="105" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="105" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A105" t="s">
         <v>112</v>
       </c>
@@ -6212,7 +6212,7 @@
         <v>760</v>
       </c>
     </row>
-    <row r="106" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="106" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A106" t="s">
         <v>113</v>
       </c>
@@ -6241,7 +6241,7 @@
         <v>760</v>
       </c>
     </row>
-    <row r="107" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="107" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A107" t="s">
         <v>114</v>
       </c>
@@ -6270,7 +6270,7 @@
         <v>760</v>
       </c>
     </row>
-    <row r="108" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="108" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A108" t="s">
         <v>115</v>
       </c>
@@ -6299,7 +6299,7 @@
         <v>760</v>
       </c>
     </row>
-    <row r="109" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="109" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A109" t="s">
         <v>116</v>
       </c>
@@ -6328,7 +6328,7 @@
         <v>760</v>
       </c>
     </row>
-    <row r="110" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="110" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A110" t="s">
         <v>117</v>
       </c>
@@ -6357,7 +6357,7 @@
         <v>888</v>
       </c>
     </row>
-    <row r="111" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="111" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A111" t="s">
         <v>118</v>
       </c>
@@ -6386,7 +6386,7 @@
         <v>760</v>
       </c>
     </row>
-    <row r="112" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="112" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A112" t="s">
         <v>119</v>
       </c>
@@ -6415,7 +6415,7 @@
         <v>760</v>
       </c>
     </row>
-    <row r="113" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="113" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A113" t="s">
         <v>120</v>
       </c>
@@ -6444,7 +6444,7 @@
         <v>760</v>
       </c>
     </row>
-    <row r="114" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="114" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A114" t="s">
         <v>121</v>
       </c>
@@ -6473,7 +6473,7 @@
         <v>760</v>
       </c>
     </row>
-    <row r="115" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="115" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A115" t="s">
         <v>122</v>
       </c>
@@ -6502,7 +6502,7 @@
         <v>760</v>
       </c>
     </row>
-    <row r="116" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="116" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A116" t="s">
         <v>123</v>
       </c>
@@ -6531,7 +6531,7 @@
         <v>760</v>
       </c>
     </row>
-    <row r="117" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="117" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A117" t="s">
         <v>124</v>
       </c>
@@ -6560,7 +6560,7 @@
         <v>760</v>
       </c>
     </row>
-    <row r="118" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="118" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A118" t="s">
         <v>125</v>
       </c>
@@ -6589,7 +6589,7 @@
         <v>760</v>
       </c>
     </row>
-    <row r="119" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="119" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A119" t="s">
         <v>126</v>
       </c>
@@ -6618,7 +6618,7 @@
         <v>760</v>
       </c>
     </row>
-    <row r="120" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="120" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A120" t="s">
         <v>127</v>
       </c>
@@ -6647,7 +6647,7 @@
         <v>760</v>
       </c>
     </row>
-    <row r="121" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="121" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A121" t="s">
         <v>128</v>
       </c>
@@ -6676,7 +6676,7 @@
         <v>760</v>
       </c>
     </row>
-    <row r="122" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="122" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A122" t="s">
         <v>129</v>
       </c>
@@ -6705,7 +6705,7 @@
         <v>760</v>
       </c>
     </row>
-    <row r="123" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="123" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A123" t="s">
         <v>130</v>
       </c>
@@ -6734,7 +6734,7 @@
         <v>760</v>
       </c>
     </row>
-    <row r="124" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="124" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A124" t="s">
         <v>131</v>
       </c>
@@ -6763,7 +6763,7 @@
         <v>760</v>
       </c>
     </row>
-    <row r="125" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="125" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A125" t="s">
         <v>132</v>
       </c>
@@ -6792,7 +6792,7 @@
         <v>888</v>
       </c>
     </row>
-    <row r="126" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="126" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A126" t="s">
         <v>133</v>
       </c>
@@ -6821,7 +6821,7 @@
         <v>760</v>
       </c>
     </row>
-    <row r="127" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="127" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A127" t="s">
         <v>134</v>
       </c>
@@ -6850,7 +6850,7 @@
         <v>760</v>
       </c>
     </row>
-    <row r="128" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="128" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A128" t="s">
         <v>135</v>
       </c>
@@ -6879,7 +6879,7 @@
         <v>760</v>
       </c>
     </row>
-    <row r="129" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="129" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A129" t="s">
         <v>136</v>
       </c>
@@ -6908,7 +6908,7 @@
         <v>760</v>
       </c>
     </row>
-    <row r="130" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="130" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A130" t="s">
         <v>137</v>
       </c>
@@ -6937,7 +6937,7 @@
         <v>760</v>
       </c>
     </row>
-    <row r="131" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="131" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A131" t="s">
         <v>138</v>
       </c>
@@ -6966,7 +6966,7 @@
         <v>760</v>
       </c>
     </row>
-    <row r="132" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="132" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A132" t="s">
         <v>139</v>
       </c>
@@ -6995,7 +6995,7 @@
         <v>892</v>
       </c>
     </row>
-    <row r="133" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="133" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A133" t="s">
         <v>140</v>
       </c>
@@ -7024,7 +7024,7 @@
         <v>760</v>
       </c>
     </row>
-    <row r="134" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="134" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A134" t="s">
         <v>141</v>
       </c>
@@ -7053,7 +7053,7 @@
         <v>888</v>
       </c>
     </row>
-    <row r="135" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="135" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A135" t="s">
         <v>142</v>
       </c>
@@ -7082,7 +7082,7 @@
         <v>760</v>
       </c>
     </row>
-    <row r="136" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="136" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A136" t="s">
         <v>143</v>
       </c>
@@ -7111,7 +7111,7 @@
         <v>760</v>
       </c>
     </row>
-    <row r="137" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="137" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A137" t="s">
         <v>144</v>
       </c>
@@ -7140,7 +7140,7 @@
         <v>760</v>
       </c>
     </row>
-    <row r="138" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="138" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A138" t="s">
         <v>145</v>
       </c>
@@ -7169,7 +7169,7 @@
         <v>760</v>
       </c>
     </row>
-    <row r="139" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="139" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A139" t="s">
         <v>146</v>
       </c>
@@ -7198,7 +7198,7 @@
         <v>760</v>
       </c>
     </row>
-    <row r="140" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="140" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A140" t="s">
         <v>147</v>
       </c>
@@ -7227,7 +7227,7 @@
         <v>760</v>
       </c>
     </row>
-    <row r="141" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="141" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A141" t="s">
         <v>148</v>
       </c>
@@ -7256,7 +7256,7 @@
         <v>893</v>
       </c>
     </row>
-    <row r="142" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="142" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A142" t="s">
         <v>149</v>
       </c>
@@ -7285,7 +7285,7 @@
         <v>760</v>
       </c>
     </row>
-    <row r="143" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="143" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A143" t="s">
         <v>150</v>
       </c>
@@ -7314,7 +7314,7 @@
         <v>760</v>
       </c>
     </row>
-    <row r="144" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="144" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A144" t="s">
         <v>151</v>
       </c>
@@ -7343,7 +7343,7 @@
         <v>760</v>
       </c>
     </row>
-    <row r="145" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="145" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A145" t="s">
         <v>152</v>
       </c>
@@ -7372,7 +7372,7 @@
         <v>760</v>
       </c>
     </row>
-    <row r="146" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="146" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A146" t="s">
         <v>153</v>
       </c>
@@ -7401,7 +7401,7 @@
         <v>894</v>
       </c>
     </row>
-    <row r="147" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="147" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A147" t="s">
         <v>154</v>
       </c>
@@ -7430,7 +7430,7 @@
         <v>760</v>
       </c>
     </row>
-    <row r="148" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="148" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A148" t="s">
         <v>155</v>
       </c>
@@ -7459,7 +7459,7 @@
         <v>760</v>
       </c>
     </row>
-    <row r="149" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="149" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A149" t="s">
         <v>156</v>
       </c>
@@ -7488,7 +7488,7 @@
         <v>760</v>
       </c>
     </row>
-    <row r="150" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="150" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A150" t="s">
         <v>157</v>
       </c>
@@ -7517,7 +7517,7 @@
         <v>760</v>
       </c>
     </row>
-    <row r="151" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="151" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A151" t="s">
         <v>158</v>
       </c>
@@ -7546,7 +7546,7 @@
         <v>760</v>
       </c>
     </row>
-    <row r="152" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="152" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A152" t="s">
         <v>159</v>
       </c>
@@ -7575,7 +7575,7 @@
         <v>760</v>
       </c>
     </row>
-    <row r="153" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="153" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A153" t="s">
         <v>160</v>
       </c>
@@ -7604,7 +7604,7 @@
         <v>760</v>
       </c>
     </row>
-    <row r="154" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="154" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A154" t="s">
         <v>161</v>
       </c>
@@ -7633,7 +7633,7 @@
         <v>760</v>
       </c>
     </row>
-    <row r="155" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="155" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A155" t="s">
         <v>162</v>
       </c>
@@ -7662,7 +7662,7 @@
         <v>760</v>
       </c>
     </row>
-    <row r="156" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="156" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A156" t="s">
         <v>163</v>
       </c>
@@ -7691,7 +7691,7 @@
         <v>760</v>
       </c>
     </row>
-    <row r="157" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="157" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A157" t="s">
         <v>164</v>
       </c>
@@ -7720,7 +7720,7 @@
         <v>760</v>
       </c>
     </row>
-    <row r="158" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="158" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A158" t="s">
         <v>165</v>
       </c>
@@ -7749,7 +7749,7 @@
         <v>760</v>
       </c>
     </row>
-    <row r="159" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="159" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A159" t="s">
         <v>166</v>
       </c>
@@ -7778,7 +7778,7 @@
         <v>760</v>
       </c>
     </row>
-    <row r="160" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="160" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A160" t="s">
         <v>167</v>
       </c>
@@ -7807,7 +7807,7 @@
         <v>760</v>
       </c>
     </row>
-    <row r="161" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="161" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A161" t="s">
         <v>168</v>
       </c>
@@ -7836,7 +7836,7 @@
         <v>760</v>
       </c>
     </row>
-    <row r="162" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="162" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A162" t="s">
         <v>169</v>
       </c>
@@ -7865,7 +7865,7 @@
         <v>760</v>
       </c>
     </row>
-    <row r="163" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="163" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A163" t="s">
         <v>170</v>
       </c>
@@ -7894,7 +7894,7 @@
         <v>760</v>
       </c>
     </row>
-    <row r="164" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="164" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A164" t="s">
         <v>171</v>
       </c>
@@ -7923,7 +7923,7 @@
         <v>760</v>
       </c>
     </row>
-    <row r="165" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="165" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A165" t="s">
         <v>172</v>
       </c>
@@ -7952,7 +7952,7 @@
         <v>760</v>
       </c>
     </row>
-    <row r="166" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="166" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A166" t="s">
         <v>173</v>
       </c>
@@ -7981,7 +7981,7 @@
         <v>760</v>
       </c>
     </row>
-    <row r="167" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="167" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A167" t="s">
         <v>174</v>
       </c>
@@ -8010,7 +8010,7 @@
         <v>893</v>
       </c>
     </row>
-    <row r="168" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="168" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A168" t="s">
         <v>175</v>
       </c>
@@ -8039,7 +8039,7 @@
         <v>760</v>
       </c>
     </row>
-    <row r="169" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="169" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A169" t="s">
         <v>176</v>
       </c>
@@ -8068,7 +8068,7 @@
         <v>760</v>
       </c>
     </row>
-    <row r="170" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="170" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A170" t="s">
         <v>177</v>
       </c>
@@ -8097,7 +8097,7 @@
         <v>760</v>
       </c>
     </row>
-    <row r="171" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="171" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A171" t="s">
         <v>178</v>
       </c>
@@ -8126,7 +8126,7 @@
         <v>760</v>
       </c>
     </row>
-    <row r="172" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="172" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A172" t="s">
         <v>179</v>
       </c>
@@ -8155,7 +8155,7 @@
         <v>760</v>
       </c>
     </row>
-    <row r="173" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="173" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A173" t="s">
         <v>180</v>
       </c>
@@ -8184,7 +8184,7 @@
         <v>760</v>
       </c>
     </row>
-    <row r="174" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="174" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A174" t="s">
         <v>181</v>
       </c>
@@ -8213,7 +8213,7 @@
         <v>760</v>
       </c>
     </row>
-    <row r="175" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="175" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A175" t="s">
         <v>182</v>
       </c>
@@ -8242,7 +8242,7 @@
         <v>760</v>
       </c>
     </row>
-    <row r="176" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="176" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A176" t="s">
         <v>183</v>
       </c>
@@ -8271,7 +8271,7 @@
         <v>760</v>
       </c>
     </row>
-    <row r="177" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="177" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A177" t="s">
         <v>184</v>
       </c>
@@ -8300,7 +8300,7 @@
         <v>760</v>
       </c>
     </row>
-    <row r="178" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="178" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A178" t="s">
         <v>185</v>
       </c>
@@ -8329,7 +8329,7 @@
         <v>760</v>
       </c>
     </row>
-    <row r="179" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="179" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A179" t="s">
         <v>186</v>
       </c>
@@ -8358,7 +8358,7 @@
         <v>760</v>
       </c>
     </row>
-    <row r="180" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="180" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A180" t="s">
         <v>187</v>
       </c>
@@ -8387,7 +8387,7 @@
         <v>760</v>
       </c>
     </row>
-    <row r="181" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="181" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A181" t="s">
         <v>188</v>
       </c>
@@ -8416,7 +8416,7 @@
         <v>760</v>
       </c>
     </row>
-    <row r="182" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="182" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A182" t="s">
         <v>189</v>
       </c>
@@ -8445,7 +8445,7 @@
         <v>760</v>
       </c>
     </row>
-    <row r="183" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="183" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A183" t="s">
         <v>190</v>
       </c>
@@ -8474,7 +8474,7 @@
         <v>760</v>
       </c>
     </row>
-    <row r="184" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="184" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A184" t="s">
         <v>191</v>
       </c>
@@ -8503,7 +8503,7 @@
         <v>760</v>
       </c>
     </row>
-    <row r="185" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="185" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A185" t="s">
         <v>192</v>
       </c>
@@ -8532,7 +8532,7 @@
         <v>760</v>
       </c>
     </row>
-    <row r="186" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="186" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A186" t="s">
         <v>193</v>
       </c>
@@ -8561,7 +8561,7 @@
         <v>760</v>
       </c>
     </row>
-    <row r="187" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="187" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A187" t="s">
         <v>194</v>
       </c>
@@ -8590,7 +8590,7 @@
         <v>760</v>
       </c>
     </row>
-    <row r="188" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="188" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A188" t="s">
         <v>195</v>
       </c>
@@ -8619,7 +8619,7 @@
         <v>760</v>
       </c>
     </row>
-    <row r="189" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="189" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A189" t="s">
         <v>196</v>
       </c>
@@ -8648,7 +8648,7 @@
         <v>760</v>
       </c>
     </row>
-    <row r="190" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="190" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A190" t="s">
         <v>197</v>
       </c>
@@ -8677,7 +8677,7 @@
         <v>760</v>
       </c>
     </row>
-    <row r="191" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="191" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A191" t="s">
         <v>198</v>
       </c>
@@ -8706,7 +8706,7 @@
         <v>760</v>
       </c>
     </row>
-    <row r="192" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="192" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A192" t="s">
         <v>199</v>
       </c>
@@ -8735,7 +8735,7 @@
         <v>760</v>
       </c>
     </row>
-    <row r="193" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="193" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A193" t="s">
         <v>200</v>
       </c>
@@ -8764,7 +8764,7 @@
         <v>760</v>
       </c>
     </row>
-    <row r="194" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="194" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A194" t="s">
         <v>201</v>
       </c>
@@ -8793,7 +8793,7 @@
         <v>760</v>
       </c>
     </row>
-    <row r="195" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="195" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A195" t="s">
         <v>202</v>
       </c>
@@ -8822,7 +8822,7 @@
         <v>760</v>
       </c>
     </row>
-    <row r="196" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="196" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A196" t="s">
         <v>203</v>
       </c>
@@ -8851,7 +8851,7 @@
         <v>760</v>
       </c>
     </row>
-    <row r="197" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="197" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A197" t="s">
         <v>204</v>
       </c>
@@ -8880,7 +8880,7 @@
         <v>760</v>
       </c>
     </row>
-    <row r="198" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="198" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A198" t="s">
         <v>205</v>
       </c>
@@ -8909,7 +8909,7 @@
         <v>760</v>
       </c>
     </row>
-    <row r="199" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="199" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A199" t="s">
         <v>206</v>
       </c>
@@ -8938,7 +8938,7 @@
         <v>760</v>
       </c>
     </row>
-    <row r="200" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="200" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A200" t="s">
         <v>207</v>
       </c>
@@ -8967,7 +8967,7 @@
         <v>760</v>
       </c>
     </row>
-    <row r="201" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="201" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A201" t="s">
         <v>208</v>
       </c>
@@ -8996,7 +8996,7 @@
         <v>760</v>
       </c>
     </row>
-    <row r="202" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="202" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A202" t="s">
         <v>209</v>
       </c>
@@ -9025,7 +9025,7 @@
         <v>760</v>
       </c>
     </row>
-    <row r="203" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="203" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A203" t="s">
         <v>210</v>
       </c>
@@ -9054,7 +9054,7 @@
         <v>760</v>
       </c>
     </row>
-    <row r="204" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="204" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A204" t="s">
         <v>211</v>
       </c>
@@ -9083,7 +9083,7 @@
         <v>760</v>
       </c>
     </row>
-    <row r="205" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="205" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A205" t="s">
         <v>212</v>
       </c>
@@ -9112,7 +9112,7 @@
         <v>895</v>
       </c>
     </row>
-    <row r="206" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="206" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A206" t="s">
         <v>213</v>
       </c>
@@ -9141,7 +9141,7 @@
         <v>760</v>
       </c>
     </row>
-    <row r="207" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="207" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A207" t="s">
         <v>214</v>
       </c>
@@ -9170,7 +9170,7 @@
         <v>760</v>
       </c>
     </row>
-    <row r="208" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="208" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A208" t="s">
         <v>215</v>
       </c>
@@ -9199,7 +9199,7 @@
         <v>760</v>
       </c>
     </row>
-    <row r="209" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="209" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A209" t="s">
         <v>216</v>
       </c>
@@ -9228,7 +9228,7 @@
         <v>760</v>
       </c>
     </row>
-    <row r="210" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="210" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A210" t="s">
         <v>217</v>
       </c>
@@ -9257,7 +9257,7 @@
         <v>760</v>
       </c>
     </row>
-    <row r="211" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="211" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A211" t="s">
         <v>218</v>
       </c>
@@ -9286,7 +9286,7 @@
         <v>760</v>
       </c>
     </row>
-    <row r="212" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="212" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A212" t="s">
         <v>219</v>
       </c>
@@ -9315,7 +9315,7 @@
         <v>760</v>
       </c>
     </row>
-    <row r="213" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="213" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A213" t="s">
         <v>220</v>
       </c>
@@ -9344,7 +9344,7 @@
         <v>760</v>
       </c>
     </row>
-    <row r="214" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="214" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A214" t="s">
         <v>221</v>
       </c>
@@ -9373,7 +9373,7 @@
         <v>760</v>
       </c>
     </row>
-    <row r="215" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="215" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A215" t="s">
         <v>222</v>
       </c>
@@ -9402,7 +9402,7 @@
         <v>896</v>
       </c>
     </row>
-    <row r="216" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="216" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A216" t="s">
         <v>223</v>
       </c>
@@ -9431,7 +9431,7 @@
         <v>760</v>
       </c>
     </row>
-    <row r="217" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="217" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A217" t="s">
         <v>224</v>
       </c>
@@ -9460,7 +9460,7 @@
         <v>760</v>
       </c>
     </row>
-    <row r="218" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="218" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A218" t="s">
         <v>225</v>
       </c>
@@ -9489,7 +9489,7 @@
         <v>760</v>
       </c>
     </row>
-    <row r="219" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="219" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A219" t="s">
         <v>226</v>
       </c>
@@ -9518,7 +9518,7 @@
         <v>760</v>
       </c>
     </row>
-    <row r="220" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="220" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A220" t="s">
         <v>227</v>
       </c>
@@ -9547,7 +9547,7 @@
         <v>760</v>
       </c>
     </row>
-    <row r="221" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="221" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A221" t="s">
         <v>228</v>
       </c>
@@ -9576,7 +9576,7 @@
         <v>760</v>
       </c>
     </row>
-    <row r="222" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="222" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A222" t="s">
         <v>229</v>
       </c>
@@ -9605,7 +9605,7 @@
         <v>760</v>
       </c>
     </row>
-    <row r="223" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="223" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A223" t="s">
         <v>230</v>
       </c>
@@ -9634,7 +9634,7 @@
         <v>760</v>
       </c>
     </row>
-    <row r="224" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="224" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A224" t="s">
         <v>231</v>
       </c>
@@ -9663,7 +9663,7 @@
         <v>760</v>
       </c>
     </row>
-    <row r="225" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="225" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A225" t="s">
         <v>232</v>
       </c>
@@ -9692,7 +9692,7 @@
         <v>897</v>
       </c>
     </row>
-    <row r="226" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="226" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A226" t="s">
         <v>233</v>
       </c>
@@ -9721,7 +9721,7 @@
         <v>760</v>
       </c>
     </row>
-    <row r="227" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="227" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A227" t="s">
         <v>234</v>
       </c>
@@ -9750,7 +9750,7 @@
         <v>760</v>
       </c>
     </row>
-    <row r="228" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="228" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A228" t="s">
         <v>235</v>
       </c>
@@ -9779,7 +9779,7 @@
         <v>760</v>
       </c>
     </row>
-    <row r="229" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="229" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A229" t="s">
         <v>236</v>
       </c>
@@ -9808,7 +9808,7 @@
         <v>760</v>
       </c>
     </row>
-    <row r="230" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="230" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A230" t="s">
         <v>237</v>
       </c>
@@ -9837,7 +9837,7 @@
         <v>760</v>
       </c>
     </row>
-    <row r="231" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="231" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A231" t="s">
         <v>238</v>
       </c>
@@ -9866,7 +9866,7 @@
         <v>760</v>
       </c>
     </row>
-    <row r="232" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="232" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A232" t="s">
         <v>239</v>
       </c>
@@ -9895,7 +9895,7 @@
         <v>760</v>
       </c>
     </row>
-    <row r="233" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="233" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A233" t="s">
         <v>240</v>
       </c>
@@ -9924,7 +9924,7 @@
         <v>760</v>
       </c>
     </row>
-    <row r="234" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="234" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A234" t="s">
         <v>241</v>
       </c>
@@ -9953,7 +9953,7 @@
         <v>760</v>
       </c>
     </row>
-    <row r="235" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="235" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A235" t="s">
         <v>242</v>
       </c>
@@ -9982,7 +9982,7 @@
         <v>760</v>
       </c>
     </row>
-    <row r="236" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="236" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A236" t="s">
         <v>243</v>
       </c>
@@ -10011,7 +10011,7 @@
         <v>760</v>
       </c>
     </row>
-    <row r="237" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="237" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A237" t="s">
         <v>244</v>
       </c>
@@ -10040,7 +10040,7 @@
         <v>888</v>
       </c>
     </row>
-    <row r="238" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="238" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A238" t="s">
         <v>245</v>
       </c>
@@ -10069,7 +10069,7 @@
         <v>760</v>
       </c>
     </row>
-    <row r="239" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="239" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A239" t="s">
         <v>246</v>
       </c>
@@ -10098,7 +10098,7 @@
         <v>760</v>
       </c>
     </row>
-    <row r="240" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="240" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A240" t="s">
         <v>247</v>
       </c>
@@ -10127,7 +10127,7 @@
         <v>760</v>
       </c>
     </row>
-    <row r="241" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="241" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A241" t="s">
         <v>248</v>
       </c>
@@ -10156,7 +10156,7 @@
         <v>760</v>
       </c>
     </row>
-    <row r="242" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="242" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A242" t="s">
         <v>249</v>
       </c>
@@ -10185,7 +10185,7 @@
         <v>760</v>
       </c>
     </row>
-    <row r="243" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="243" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A243" t="s">
         <v>250</v>
       </c>
@@ -10214,7 +10214,7 @@
         <v>760</v>
       </c>
     </row>
-    <row r="244" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="244" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A244" t="s">
         <v>251</v>
       </c>
@@ -10243,7 +10243,7 @@
         <v>760</v>
       </c>
     </row>
-    <row r="245" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="245" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A245" t="s">
         <v>252</v>
       </c>
@@ -10272,7 +10272,7 @@
         <v>760</v>
       </c>
     </row>
-    <row r="246" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="246" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A246" t="s">
         <v>253</v>
       </c>
@@ -10301,7 +10301,7 @@
         <v>760</v>
       </c>
     </row>
-    <row r="247" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="247" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A247" t="s">
         <v>254</v>
       </c>
@@ -10330,7 +10330,7 @@
         <v>898</v>
       </c>
     </row>
-    <row r="248" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="248" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A248" t="s">
         <v>255</v>
       </c>
@@ -10359,7 +10359,7 @@
         <v>760</v>
       </c>
     </row>
-    <row r="249" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="249" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A249" t="s">
         <v>256</v>
       </c>
@@ -10388,7 +10388,7 @@
         <v>760</v>
       </c>
     </row>
-    <row r="250" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="250" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A250" t="s">
         <v>257</v>
       </c>
@@ -10417,7 +10417,7 @@
         <v>760</v>
       </c>
     </row>
-    <row r="251" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="251" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A251" t="s">
         <v>258</v>
       </c>
@@ -10446,7 +10446,7 @@
         <v>888</v>
       </c>
     </row>
-    <row r="252" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="252" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A252" t="s">
         <v>259</v>
       </c>
@@ -10475,7 +10475,7 @@
         <v>760</v>
       </c>
     </row>
-    <row r="253" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="253" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A253" t="s">
         <v>260</v>
       </c>
@@ -10504,7 +10504,7 @@
         <v>760</v>
       </c>
     </row>
-    <row r="254" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="254" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A254" t="s">
         <v>261</v>
       </c>
@@ -10533,7 +10533,7 @@
         <v>760</v>
       </c>
     </row>
-    <row r="255" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="255" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A255" t="s">
         <v>262</v>
       </c>
@@ -10562,7 +10562,7 @@
         <v>760</v>
       </c>
     </row>
-    <row r="256" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="256" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A256" t="s">
         <v>263</v>
       </c>
@@ -10591,7 +10591,7 @@
         <v>760</v>
       </c>
     </row>
-    <row r="257" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="257" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A257" t="s">
         <v>264</v>
       </c>
@@ -10620,7 +10620,7 @@
         <v>760</v>
       </c>
     </row>
-    <row r="258" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="258" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A258" t="s">
         <v>265</v>
       </c>
@@ -10649,7 +10649,7 @@
         <v>760</v>
       </c>
     </row>
-    <row r="259" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="259" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A259" t="s">
         <v>266</v>
       </c>
@@ -10678,7 +10678,7 @@
         <v>760</v>
       </c>
     </row>
-    <row r="260" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="260" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A260" t="s">
         <v>267</v>
       </c>
@@ -10707,7 +10707,7 @@
         <v>760</v>
       </c>
     </row>
-    <row r="261" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="261" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A261" t="s">
         <v>268</v>
       </c>
@@ -10736,7 +10736,7 @@
         <v>886</v>
       </c>
     </row>
-    <row r="262" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="262" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A262" t="s">
         <v>269</v>
       </c>
@@ -10765,7 +10765,7 @@
         <v>760</v>
       </c>
     </row>
-    <row r="263" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="263" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A263" t="s">
         <v>270</v>
       </c>
@@ -10794,7 +10794,7 @@
         <v>760</v>
       </c>
     </row>
-    <row r="264" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="264" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A264" t="s">
         <v>271</v>
       </c>
@@ -10823,7 +10823,7 @@
         <v>897</v>
       </c>
     </row>
-    <row r="265" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="265" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A265" t="s">
         <v>272</v>
       </c>
@@ -10852,7 +10852,7 @@
         <v>760</v>
       </c>
     </row>
-    <row r="266" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="266" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A266" t="s">
         <v>273</v>
       </c>
@@ -10881,7 +10881,7 @@
         <v>899</v>
       </c>
     </row>
-    <row r="267" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="267" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A267" t="s">
         <v>274</v>
       </c>
@@ -10910,7 +10910,7 @@
         <v>900</v>
       </c>
     </row>
-    <row r="268" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="268" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A268" t="s">
         <v>275</v>
       </c>
@@ -10939,7 +10939,7 @@
         <v>760</v>
       </c>
     </row>
-    <row r="269" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="269" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A269" t="s">
         <v>276</v>
       </c>
@@ -10968,7 +10968,7 @@
         <v>760</v>
       </c>
     </row>
-    <row r="270" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="270" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A270" t="s">
         <v>277</v>
       </c>
@@ -10997,7 +10997,7 @@
         <v>760</v>
       </c>
     </row>
-    <row r="271" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="271" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A271" t="s">
         <v>278</v>
       </c>
@@ -11026,7 +11026,7 @@
         <v>897</v>
       </c>
     </row>
-    <row r="272" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="272" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A272" t="s">
         <v>279</v>
       </c>
@@ -11055,7 +11055,7 @@
         <v>760</v>
       </c>
     </row>
-    <row r="273" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="273" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A273" t="s">
         <v>280</v>
       </c>
@@ -11084,7 +11084,7 @@
         <v>760</v>
       </c>
     </row>
-    <row r="274" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="274" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A274" t="s">
         <v>281</v>
       </c>
@@ -11113,7 +11113,7 @@
         <v>760</v>
       </c>
     </row>
-    <row r="275" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="275" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A275" t="s">
         <v>94</v>
       </c>
@@ -11142,7 +11142,7 @@
         <v>760</v>
       </c>
     </row>
-    <row r="276" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="276" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A276" t="s">
         <v>282</v>
       </c>
@@ -11171,7 +11171,7 @@
         <v>760</v>
       </c>
     </row>
-    <row r="277" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="277" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A277" t="s">
         <v>283</v>
       </c>
@@ -11200,7 +11200,7 @@
         <v>760</v>
       </c>
     </row>
-    <row r="278" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="278" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A278" t="s">
         <v>284</v>
       </c>
@@ -11229,7 +11229,7 @@
         <v>760</v>
       </c>
     </row>
-    <row r="279" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="279" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A279" t="s">
         <v>285</v>
       </c>
@@ -11258,7 +11258,7 @@
         <v>760</v>
       </c>
     </row>
-    <row r="280" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="280" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A280" t="s">
         <v>286</v>
       </c>
@@ -11287,7 +11287,7 @@
         <v>760</v>
       </c>
     </row>
-    <row r="281" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="281" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A281" t="s">
         <v>287</v>
       </c>
@@ -11316,7 +11316,7 @@
         <v>760</v>
       </c>
     </row>
-    <row r="282" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="282" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A282" t="s">
         <v>288</v>
       </c>
@@ -11345,7 +11345,7 @@
         <v>760</v>
       </c>
     </row>
-    <row r="283" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="283" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A283" t="s">
         <v>289</v>
       </c>
@@ -11374,7 +11374,7 @@
         <v>760</v>
       </c>
     </row>
-    <row r="284" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="284" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A284" t="s">
         <v>290</v>
       </c>
@@ -11403,7 +11403,7 @@
         <v>901</v>
       </c>
     </row>
-    <row r="285" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="285" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A285" t="s">
         <v>291</v>
       </c>
@@ -11432,7 +11432,7 @@
         <v>760</v>
       </c>
     </row>
-    <row r="286" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="286" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A286" t="s">
         <v>292</v>
       </c>
@@ -11461,7 +11461,7 @@
         <v>760</v>
       </c>
     </row>
-    <row r="287" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="287" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A287" t="s">
         <v>293</v>
       </c>
@@ -11490,7 +11490,7 @@
         <v>902</v>
       </c>
     </row>
-    <row r="288" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="288" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A288" t="s">
         <v>294</v>
       </c>
@@ -11519,7 +11519,7 @@
         <v>760</v>
       </c>
     </row>
-    <row r="289" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="289" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A289" t="s">
         <v>295</v>
       </c>
@@ -11548,7 +11548,7 @@
         <v>760</v>
       </c>
     </row>
-    <row r="290" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="290" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A290" t="s">
         <v>296</v>
       </c>
@@ -11577,7 +11577,7 @@
         <v>903</v>
       </c>
     </row>
-    <row r="291" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="291" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A291" t="s">
         <v>297</v>
       </c>
@@ -11606,7 +11606,7 @@
         <v>760</v>
       </c>
     </row>
-    <row r="292" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="292" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A292" t="s">
         <v>298</v>
       </c>
@@ -11635,7 +11635,7 @@
         <v>760</v>
       </c>
     </row>
-    <row r="293" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="293" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A293" t="s">
         <v>299</v>
       </c>
@@ -11664,7 +11664,7 @@
         <v>904</v>
       </c>
     </row>
-    <row r="294" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="294" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A294" t="s">
         <v>300</v>
       </c>
@@ -11693,7 +11693,7 @@
         <v>760</v>
       </c>
     </row>
-    <row r="295" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="295" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A295" t="s">
         <v>301</v>
       </c>
@@ -11722,7 +11722,7 @@
         <v>760</v>
       </c>
     </row>
-    <row r="296" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="296" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A296" t="s">
         <v>302</v>
       </c>
@@ -11751,7 +11751,7 @@
         <v>760</v>
       </c>
     </row>
-    <row r="297" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="297" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A297" t="s">
         <v>303</v>
       </c>
@@ -11774,7 +11774,7 @@
         <v>912</v>
       </c>
     </row>
-    <row r="298" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="298" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A298" t="s">
         <v>304</v>
       </c>
@@ -11803,7 +11803,7 @@
         <v>905</v>
       </c>
     </row>
-    <row r="299" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="299" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A299" t="s">
         <v>305</v>
       </c>
@@ -11832,7 +11832,7 @@
         <v>888</v>
       </c>
     </row>
-    <row r="300" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="300" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A300" t="s">
         <v>913</v>
       </c>
@@ -11852,7 +11852,7 @@
         <v>914</v>
       </c>
     </row>
-    <row r="301" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="301" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A301" t="s">
         <v>306</v>
       </c>
@@ -11881,7 +11881,7 @@
         <v>760</v>
       </c>
     </row>
-    <row r="302" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="302" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A302" t="s">
         <v>307</v>
       </c>
@@ -11910,7 +11910,7 @@
         <v>760</v>
       </c>
     </row>
-    <row r="303" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="303" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A303" t="s">
         <v>308</v>
       </c>
@@ -11939,7 +11939,7 @@
         <v>760</v>
       </c>
     </row>
-    <row r="304" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="304" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A304" t="s">
         <v>309</v>
       </c>
@@ -11968,7 +11968,7 @@
         <v>760</v>
       </c>
     </row>
-    <row r="305" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="305" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A305" t="s">
         <v>310</v>
       </c>
@@ -11997,7 +11997,7 @@
         <v>906</v>
       </c>
     </row>
-    <row r="306" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="306" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A306" t="s">
         <v>311</v>
       </c>
@@ -12026,7 +12026,7 @@
         <v>888</v>
       </c>
     </row>
-    <row r="307" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="307" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A307" t="s">
         <v>312</v>
       </c>
@@ -12055,7 +12055,7 @@
         <v>905</v>
       </c>
     </row>
-    <row r="308" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="308" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A308" t="s">
         <v>313</v>
       </c>
@@ -12078,7 +12078,7 @@
         <v>916</v>
       </c>
     </row>
-    <row r="309" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="309" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A309" t="s">
         <v>314</v>
       </c>
@@ -12107,7 +12107,7 @@
         <v>760</v>
       </c>
     </row>
-    <row r="310" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="310" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A310" t="s">
         <v>315</v>
       </c>
@@ -12136,7 +12136,7 @@
         <v>888</v>
       </c>
     </row>
-    <row r="311" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="311" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A311" t="s">
         <v>316</v>
       </c>
@@ -12165,7 +12165,7 @@
         <v>895</v>
       </c>
     </row>
-    <row r="312" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="312" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A312" t="s">
         <v>317</v>
       </c>
@@ -12194,7 +12194,7 @@
         <v>760</v>
       </c>
     </row>
-    <row r="313" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="313" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A313" t="s">
         <v>318</v>
       </c>
@@ -12223,7 +12223,7 @@
         <v>760</v>
       </c>
     </row>
-    <row r="314" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="314" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A314" t="s">
         <v>319</v>
       </c>
@@ -12252,7 +12252,7 @@
         <v>896</v>
       </c>
     </row>
-    <row r="315" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="315" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A315" t="s">
         <v>320</v>
       </c>
@@ -12281,7 +12281,7 @@
         <v>760</v>
       </c>
     </row>
-    <row r="316" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="316" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A316" t="s">
         <v>321</v>
       </c>
@@ -12310,7 +12310,7 @@
         <v>907</v>
       </c>
     </row>
-    <row r="317" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="317" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A317" t="s">
         <v>322</v>
       </c>
@@ -12339,7 +12339,7 @@
         <v>760</v>
       </c>
     </row>
-    <row r="318" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="318" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A318" t="s">
         <v>323</v>
       </c>
@@ -12368,7 +12368,7 @@
         <v>760</v>
       </c>
     </row>
-    <row r="319" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="319" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A319" t="s">
         <v>324</v>
       </c>
@@ -12397,7 +12397,7 @@
         <v>760</v>
       </c>
     </row>
-    <row r="320" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="320" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A320" t="s">
         <v>325</v>
       </c>
@@ -12426,7 +12426,7 @@
         <v>760</v>
       </c>
     </row>
-    <row r="321" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="321" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A321" t="s">
         <v>326</v>
       </c>
@@ -12455,7 +12455,7 @@
         <v>760</v>
       </c>
     </row>
-    <row r="322" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="322" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A322" t="s">
         <v>327</v>
       </c>
@@ -12484,7 +12484,7 @@
         <v>760</v>
       </c>
     </row>
-    <row r="323" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="323" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A323" t="s">
         <v>328</v>
       </c>
@@ -12513,7 +12513,7 @@
         <v>760</v>
       </c>
     </row>
-    <row r="324" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="324" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A324" t="s">
         <v>329</v>
       </c>
@@ -12542,7 +12542,7 @@
         <v>760</v>
       </c>
     </row>
-    <row r="325" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="325" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A325" t="s">
         <v>330</v>
       </c>
@@ -12571,7 +12571,7 @@
         <v>760</v>
       </c>
     </row>
-    <row r="326" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="326" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A326" t="s">
         <v>331</v>
       </c>
@@ -12600,7 +12600,7 @@
         <v>760</v>
       </c>
     </row>
-    <row r="327" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="327" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A327" t="s">
         <v>332</v>
       </c>
@@ -12629,7 +12629,7 @@
         <v>760</v>
       </c>
     </row>
-    <row r="328" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="328" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A328" t="s">
         <v>333</v>
       </c>
@@ -12658,7 +12658,7 @@
         <v>760</v>
       </c>
     </row>
-    <row r="329" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="329" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A329" t="s">
         <v>334</v>
       </c>
@@ -12687,7 +12687,7 @@
         <v>760</v>
       </c>
     </row>
-    <row r="330" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="330" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A330" t="s">
         <v>335</v>
       </c>
@@ -12716,7 +12716,7 @@
         <v>760</v>
       </c>
     </row>
-    <row r="331" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="331" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A331" t="s">
         <v>336</v>
       </c>
@@ -12745,7 +12745,7 @@
         <v>760</v>
       </c>
     </row>
-    <row r="332" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="332" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A332" t="s">
         <v>337</v>
       </c>
@@ -12774,7 +12774,7 @@
         <v>760</v>
       </c>
     </row>
-    <row r="333" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="333" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A333" t="s">
         <v>338</v>
       </c>
@@ -12803,7 +12803,7 @@
         <v>760</v>
       </c>
     </row>
-    <row r="334" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="334" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A334" t="s">
         <v>339</v>
       </c>
@@ -12832,7 +12832,7 @@
         <v>760</v>
       </c>
     </row>
-    <row r="335" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="335" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A335" t="s">
         <v>340</v>
       </c>
@@ -12861,7 +12861,7 @@
         <v>760</v>
       </c>
     </row>
-    <row r="336" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="336" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A336" t="s">
         <v>341</v>
       </c>
@@ -12890,7 +12890,7 @@
         <v>760</v>
       </c>
     </row>
-    <row r="337" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="337" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A337" t="s">
         <v>342</v>
       </c>
@@ -12919,7 +12919,7 @@
         <v>760</v>
       </c>
     </row>
-    <row r="338" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="338" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A338" t="s">
         <v>343</v>
       </c>
@@ -12948,7 +12948,7 @@
         <v>760</v>
       </c>
     </row>
-    <row r="339" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="339" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A339" t="s">
         <v>344</v>
       </c>
@@ -12977,7 +12977,7 @@
         <v>760</v>
       </c>
     </row>
-    <row r="340" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="340" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A340" t="s">
         <v>345</v>
       </c>
@@ -13006,7 +13006,7 @@
         <v>760</v>
       </c>
     </row>
-    <row r="341" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="341" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A341" t="s">
         <v>346</v>
       </c>
@@ -13035,7 +13035,7 @@
         <v>760</v>
       </c>
     </row>
-    <row r="342" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="342" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A342" t="s">
         <v>347</v>
       </c>
@@ -13064,7 +13064,7 @@
         <v>760</v>
       </c>
     </row>
-    <row r="343" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="343" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A343" t="s">
         <v>348</v>
       </c>
@@ -13093,7 +13093,7 @@
         <v>760</v>
       </c>
     </row>
-    <row r="344" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="344" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A344" t="s">
         <v>349</v>
       </c>
@@ -13122,7 +13122,7 @@
         <v>760</v>
       </c>
     </row>
-    <row r="345" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="345" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A345" t="s">
         <v>350</v>
       </c>
@@ -13151,7 +13151,7 @@
         <v>760</v>
       </c>
     </row>
-    <row r="346" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="346" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A346" t="s">
         <v>351</v>
       </c>
@@ -13180,7 +13180,7 @@
         <v>760</v>
       </c>
     </row>
-    <row r="347" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="347" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A347" t="s">
         <v>352</v>
       </c>
@@ -13209,7 +13209,7 @@
         <v>760</v>
       </c>
     </row>
-    <row r="348" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="348" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A348" t="s">
         <v>353</v>
       </c>
@@ -13238,7 +13238,7 @@
         <v>760</v>
       </c>
     </row>
-    <row r="349" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="349" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A349" t="s">
         <v>354</v>
       </c>
@@ -13267,7 +13267,7 @@
         <v>760</v>
       </c>
     </row>
-    <row r="350" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="350" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A350" t="s">
         <v>355</v>
       </c>
@@ -13296,7 +13296,7 @@
         <v>760</v>
       </c>
     </row>
-    <row r="351" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="351" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A351" t="s">
         <v>356</v>
       </c>

</xml_diff>